<commit_message>
Clip Uranus data anomaly
</commit_message>
<xml_diff>
--- a/interplanetary-data/Uranus/U3.xlsx
+++ b/interplanetary-data/Uranus/U3.xlsx
@@ -13,10 +13,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1591621747" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1591621747" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1591621747" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1591621747"/>
+      <pm:revision xmlns:pm="smNativeData" day="1591622550" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1591622550" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1591622550" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1591622550"/>
     </ext>
   </extLst>
 </workbook>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">   %path</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t xml:space="preserve">       Lmass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Acdate</t>
   </si>
   <si>
     <t>Atof</t>
@@ -91,7 +88,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591621747" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1591622550" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -106,7 +103,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1591621747" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1591622550" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -124,22 +121,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE1EFD8"/>
+        <fgColor rgb="FFFDE9D9"/>
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591621747" type="1" fgLvl="100" fgClr="00E1EFD8" bgLvl="100" bgClr="00E1EFD8"/>
+            <pm:shade xmlns:pm="smNativeData" id="1591622550" type="1" fgLvl="100" fgClr="00FDE9D9" bgLvl="100" bgClr="00FDE9D9"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
+        <fgColor rgb="FFF79646"/>
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1591621747" type="1" fgLvl="100" fgClr="0070AD47" bgLvl="100" bgClr="0070AD47"/>
+            <pm:shade xmlns:pm="smNativeData" id="1591622550" type="1" fgLvl="100" fgClr="00F79646" bgLvl="100" bgClr="00F79646"/>
           </ext>
         </extLst>
       </patternFill>
@@ -161,7 +158,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591621747"/>
+          <pm:border xmlns:pm="smNativeData" id="1591622550"/>
         </ext>
       </extLst>
     </border>
@@ -180,7 +177,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591621747"/>
+          <pm:border xmlns:pm="smNativeData" id="1591622550"/>
         </ext>
       </extLst>
     </border>
@@ -199,7 +196,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1591621747"/>
+          <pm:border xmlns:pm="smNativeData" id="1591622550"/>
         </ext>
       </extLst>
     </border>
@@ -216,13 +213,16 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1591621747" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1591622550" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1591621747" count="3">
+      <pm:colors xmlns:pm="smNativeData" id="1591622550" count="6">
         <pm:color name="Color 24" rgb="A8D08C"/>
         <pm:color name="Color 25" rgb="70AD47"/>
         <pm:color name="Color 26" rgb="E1EFD8"/>
+        <pm:color name="Color 27" rgb="FABF8F"/>
+        <pm:color name="Color 28" rgb="F79646"/>
+        <pm:color name="Color 29" rgb="FDE9D9"/>
       </pm:colors>
     </ext>
   </extLst>
@@ -230,21 +230,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="res" displayName="res" ref="A1:L109" totalsRowShown="0">
-  <autoFilter ref="A1:L109"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="res" displayName="res" ref="A1:K109" totalsRowShown="0">
+  <autoFilter ref="A1:K109"/>
+  <tableColumns count="11">
     <tableColumn id="1" name="   %path" totalsRowLabel="Total"/>
     <tableColumn id="2" name="LC3"/>
     <tableColumn id="3" name="              Ldec"/>
     <tableColumn id="4" name="       Lmass"/>
-    <tableColumn id="5" name="    Acdate"/>
-    <tableColumn id="6" name="Atof"/>
-    <tableColumn id="7" name="Avinf"/>
-    <tableColumn id="8" name="              Adec"/>
-    <tableColumn id="9" name="     Amass"/>
-    <tableColumn id="10" name="             AoiDM"/>
-    <tableColumn id="11" name="             AoiDV"/>
-    <tableColumn id="12" name="  EPprop"/>
+    <tableColumn id="5" name="Atof"/>
+    <tableColumn id="6" name="Avinf"/>
+    <tableColumn id="7" name="              Adec"/>
+    <tableColumn id="8" name="     Amass"/>
+    <tableColumn id="9" name="             AoiDM"/>
+    <tableColumn id="10" name="             AoiDV"/>
+    <tableColumn id="11" name="  EPprop" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -506,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R109"/>
+  <dimension ref="A1:L109"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -518,17 +517,16 @@
     <col min="2" max="2" width="12.857143" customWidth="1"/>
     <col min="3" max="3" width="13.142857" customWidth="1"/>
     <col min="4" max="4" width="11.428571" customWidth="1"/>
-    <col min="5" max="5" width="10.714286" customWidth="1"/>
-    <col min="6" max="6" width="10.428571" customWidth="1"/>
-    <col min="7" max="7" width="13.285714" customWidth="1"/>
-    <col min="8" max="8" width="13.571429" customWidth="1"/>
-    <col min="9" max="9" width="10.857143" customWidth="1"/>
-    <col min="10" max="10" width="14.714286" customWidth="1"/>
-    <col min="11" max="11" width="14.142857" customWidth="1"/>
-    <col min="12" max="12" width="10.142857" customWidth="1"/>
+    <col min="5" max="5" width="10.428571" customWidth="1"/>
+    <col min="6" max="6" width="13.285714" customWidth="1"/>
+    <col min="7" max="7" width="13.571429" customWidth="1"/>
+    <col min="8" max="8" width="10.857143" customWidth="1"/>
+    <col min="9" max="9" width="14.714286" customWidth="1"/>
+    <col min="10" max="10" width="14.142857" customWidth="1"/>
+    <col min="11" max="11" width="10.142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -562,11 +560,8 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="n">
         <v>33357</v>
       </c>
@@ -580,31 +575,28 @@
         <v>5788.98829999999998</v>
       </c>
       <c r="E2" t="n">
-        <v>20410408</v>
+        <v>4017.75</v>
       </c>
       <c r="F2" t="n">
-        <v>4017.75</v>
+        <v>12.1825469999999996</v>
       </c>
       <c r="G2" t="n">
-        <v>12.1825469999999996</v>
+        <v>47.4847499999999982</v>
       </c>
       <c r="H2" t="n">
-        <v>47.4847499999999982</v>
+        <v>1539.36740000000009</v>
       </c>
       <c r="I2" t="n">
-        <v>1539.36740000000009</v>
+        <v>2962.61760000000004</v>
       </c>
       <c r="J2" t="n">
-        <v>2962.61760000000004</v>
+        <v>3.42029210000000017</v>
       </c>
       <c r="K2" t="n">
-        <v>3.42029210000000017</v>
-      </c>
-      <c r="L2" t="n">
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:12">
       <c r="A3" t="n">
         <v>33357</v>
       </c>
@@ -618,31 +610,28 @@
         <v>4402.02940000000035</v>
       </c>
       <c r="E3" t="n">
-        <v>20400723</v>
+        <v>4017.75</v>
       </c>
       <c r="F3" t="n">
-        <v>4017.75</v>
+        <v>13.9885710000000003</v>
       </c>
       <c r="G3" t="n">
-        <v>13.9885710000000003</v>
+        <v>48.564512999999998</v>
       </c>
       <c r="H3" t="n">
-        <v>48.564512999999998</v>
+        <v>837.925399999999854</v>
       </c>
       <c r="I3" t="n">
-        <v>837.925399999999854</v>
+        <v>2489.92250000000013</v>
       </c>
       <c r="J3" t="n">
-        <v>2489.92250000000013</v>
+        <v>4.39557969999999987</v>
       </c>
       <c r="K3" t="n">
-        <v>4.39557969999999987</v>
-      </c>
-      <c r="L3" t="n">
         <v>324.199999999999989</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:12">
       <c r="A4" t="n">
         <v>33357</v>
       </c>
@@ -656,31 +645,28 @@
         <v>5792.86520000000019</v>
       </c>
       <c r="E4" t="n">
-        <v>20410408</v>
+        <v>4017.75</v>
       </c>
       <c r="F4" t="n">
-        <v>4017.75</v>
+        <v>12.18126</v>
       </c>
       <c r="G4" t="n">
-        <v>12.18126</v>
+        <v>47.4840710000000001</v>
       </c>
       <c r="H4" t="n">
-        <v>47.4840710000000001</v>
+        <v>1539.75559999999996</v>
       </c>
       <c r="I4" t="n">
-        <v>1539.75559999999996</v>
+        <v>2962.43159999999989</v>
       </c>
       <c r="J4" t="n">
-        <v>2962.43159999999989</v>
+        <v>3.41963149999999994</v>
       </c>
       <c r="K4" t="n">
-        <v>3.41963149999999994</v>
-      </c>
-      <c r="L4" t="n">
         <v>540.700000000000045</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:12">
       <c r="A5" t="n">
         <v>33357</v>
       </c>
@@ -694,31 +680,28 @@
         <v>5851.67569999999978</v>
       </c>
       <c r="E5" t="n">
-        <v>20410614</v>
+        <v>4017.75</v>
       </c>
       <c r="F5" t="n">
-        <v>4017.75</v>
+        <v>11.7442849999999996</v>
       </c>
       <c r="G5" t="n">
-        <v>11.7442849999999996</v>
+        <v>47.2783760000000015</v>
       </c>
       <c r="H5" t="n">
-        <v>47.2783760000000015</v>
+        <v>1658.84079999999994</v>
       </c>
       <c r="I5" t="n">
-        <v>1658.84079999999994</v>
+        <v>2866.33789999999999</v>
       </c>
       <c r="J5" t="n">
-        <v>2866.33789999999999</v>
+        <v>3.19843739999999999</v>
       </c>
       <c r="K5" t="n">
-        <v>3.19843739999999999</v>
-      </c>
-      <c r="L5" t="n">
         <v>576.5</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:12">
       <c r="A6" t="n">
         <v>33357</v>
       </c>
@@ -732,31 +715,28 @@
         <v>5667.70830000000024</v>
       </c>
       <c r="E6" t="n">
-        <v>20400710</v>
+        <v>3652.5</v>
       </c>
       <c r="F6" t="n">
-        <v>3652.5</v>
+        <v>14.0876009999999994</v>
       </c>
       <c r="G6" t="n">
-        <v>14.0876009999999994</v>
+        <v>48.6243529999999993</v>
       </c>
       <c r="H6" t="n">
-        <v>48.6243529999999993</v>
+        <v>1067.39869999999996</v>
       </c>
       <c r="I6" t="n">
-        <v>1067.39869999999996</v>
+        <v>3247.18940000000021</v>
       </c>
       <c r="J6" t="n">
-        <v>3247.18940000000021</v>
+        <v>4.45175449999999984</v>
       </c>
       <c r="K6" t="n">
-        <v>4.45175449999999984</v>
-      </c>
-      <c r="L6" t="n">
         <v>603.100000000000023</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:12">
       <c r="A7" t="n">
         <v>33357</v>
       </c>
@@ -770,31 +750,28 @@
         <v>5819.91690000000017</v>
       </c>
       <c r="E7" t="n">
-        <v>20410624</v>
+        <v>4017.75</v>
       </c>
       <c r="F7" t="n">
-        <v>4017.75</v>
+        <v>11.6835070000000005</v>
       </c>
       <c r="G7" t="n">
-        <v>11.6835070000000005</v>
+        <v>47.2470720000000028</v>
       </c>
       <c r="H7" t="n">
-        <v>47.2470720000000028</v>
+        <v>1672.9996000000001</v>
       </c>
       <c r="I7" t="n">
-        <v>1672.9996000000001</v>
+        <v>2847.63999999999987</v>
       </c>
       <c r="J7" t="n">
-        <v>2847.63999999999987</v>
+        <v>3.16815079999999982</v>
       </c>
       <c r="K7" t="n">
-        <v>3.16815079999999982</v>
-      </c>
-      <c r="L7" t="n">
         <v>549.299999999999955</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:12">
       <c r="A8" t="n">
         <v>33357</v>
       </c>
@@ -808,31 +785,28 @@
         <v>5784.51170000000002</v>
       </c>
       <c r="E8" t="n">
-        <v>20410407</v>
+        <v>4017.75</v>
       </c>
       <c r="F8" t="n">
-        <v>4017.75</v>
+        <v>12.1854410000000009</v>
       </c>
       <c r="G8" t="n">
-        <v>12.1854410000000009</v>
+        <v>47.486106999999997</v>
       </c>
       <c r="H8" t="n">
-        <v>47.486106999999997</v>
+        <v>1538.58200000000011</v>
       </c>
       <c r="I8" t="n">
-        <v>1538.58200000000011</v>
+        <v>2963.20280000000002</v>
       </c>
       <c r="J8" t="n">
-        <v>2963.20280000000002</v>
+        <v>3.42177689999999979</v>
       </c>
       <c r="K8" t="n">
-        <v>3.42177689999999979</v>
-      </c>
-      <c r="L8" t="n">
         <v>532.700000000000045</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:12">
       <c r="A9" t="n">
         <v>33357</v>
       </c>
@@ -846,31 +820,28 @@
         <v>5818.1297999999997</v>
       </c>
       <c r="E9" t="n">
-        <v>20410624</v>
+        <v>4017.75</v>
       </c>
       <c r="F9" t="n">
-        <v>4017.75</v>
+        <v>11.6847540000000016</v>
       </c>
       <c r="G9" t="n">
-        <v>11.6847539999999999</v>
+        <v>47.2475659999999991</v>
       </c>
       <c r="H9" t="n">
-        <v>47.2475659999999991</v>
+        <v>1672.52389999999991</v>
       </c>
       <c r="I9" t="n">
-        <v>1672.52389999999991</v>
+        <v>2847.70980000000009</v>
       </c>
       <c r="J9" t="n">
-        <v>2847.70980000000009</v>
+        <v>3.168771</v>
       </c>
       <c r="K9" t="n">
-        <v>3.168771</v>
-      </c>
-      <c r="L9" t="n">
         <v>547.899999999999977</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:12">
       <c r="A10" t="n">
         <v>33357</v>
       </c>
@@ -884,31 +855,28 @@
         <v>5817.59959999999955</v>
       </c>
       <c r="E10" t="n">
-        <v>20410624</v>
+        <v>4017.75</v>
       </c>
       <c r="F10" t="n">
-        <v>4017.75</v>
+        <v>11.6850459999999998</v>
       </c>
       <c r="G10" t="n">
-        <v>11.6850459999999998</v>
+        <v>47.247793999999999</v>
       </c>
       <c r="H10" t="n">
-        <v>47.247793999999999</v>
+        <v>1672.79739999999993</v>
       </c>
       <c r="I10" t="n">
-        <v>1672.79739999999993</v>
+        <v>2848.38110000000006</v>
       </c>
       <c r="J10" t="n">
-        <v>2848.38110000000006</v>
+        <v>3.16891599999999984</v>
       </c>
       <c r="K10" t="n">
-        <v>3.16891599999999984</v>
-      </c>
-      <c r="L10" t="n">
         <v>546.399999999999977</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:12">
       <c r="A11" t="n">
         <v>33357</v>
       </c>
@@ -922,31 +890,28 @@
         <v>3752.06059999999979</v>
       </c>
       <c r="E11" t="n">
-        <v>20410721</v>
+        <v>4017.75</v>
       </c>
       <c r="F11" t="n">
-        <v>4017.75</v>
+        <v>11.5237420000000004</v>
       </c>
       <c r="G11" t="n">
-        <v>11.5237420000000004</v>
+        <v>47.1626800000000017</v>
       </c>
       <c r="H11" t="n">
-        <v>47.1626800000000017</v>
+        <v>883.045499999999834</v>
       </c>
       <c r="I11" t="n">
-        <v>883.045499999999834</v>
+        <v>1444.59429999999998</v>
       </c>
       <c r="J11" t="n">
-        <v>1444.59429999999998</v>
+        <v>3.08910280000000004</v>
       </c>
       <c r="K11" t="n">
-        <v>3.08910280000000004</v>
-      </c>
-      <c r="L11" t="n">
         <v>674.399999999999977</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:12">
       <c r="A12" t="n">
         <v>33357</v>
       </c>
@@ -960,31 +925,28 @@
         <v>3531.48010000000022</v>
       </c>
       <c r="E12" t="n">
-        <v>20400813</v>
+        <v>3652.5</v>
       </c>
       <c r="F12" t="n">
-        <v>3652.5</v>
+        <v>13.8492189999999997</v>
       </c>
       <c r="G12" t="n">
-        <v>13.8492189999999997</v>
+        <v>48.4340369999999965</v>
       </c>
       <c r="H12" t="n">
-        <v>48.4340369999999965</v>
+        <v>567.183400000000006</v>
       </c>
       <c r="I12" t="n">
-        <v>567.183400000000006</v>
+        <v>1630.53700000000003</v>
       </c>
       <c r="J12" t="n">
-        <v>1630.53700000000003</v>
+        <v>4.31698839999999961</v>
       </c>
       <c r="K12" t="n">
-        <v>4.31698839999999961</v>
-      </c>
-      <c r="L12" t="n">
         <v>583.799999999999955</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:12">
       <c r="A13" t="n">
         <v>33357</v>
       </c>
@@ -998,31 +960,28 @@
         <v>4507.32290000000012</v>
       </c>
       <c r="E13" t="n">
-        <v>20421004</v>
+        <v>4017.75</v>
       </c>
       <c r="F13" t="n">
-        <v>4017.75</v>
+        <v>10.1137630000000005</v>
       </c>
       <c r="G13" t="n">
-        <v>10.1137630000000005</v>
+        <v>50.8597460000000012</v>
       </c>
       <c r="H13" t="n">
-        <v>50.8597460000000012</v>
+        <v>1552.84529999999995</v>
       </c>
       <c r="I13" t="n">
-        <v>1552.84529999999995</v>
+        <v>1773.82490000000007</v>
       </c>
       <c r="J13" t="n">
-        <v>1773.82490000000007</v>
+        <v>2.42824380000000017</v>
       </c>
       <c r="K13" t="n">
-        <v>2.42824380000000017</v>
-      </c>
-      <c r="L13" t="n">
         <v>430.699999999999989</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:12">
       <c r="A14" t="n">
         <v>33357</v>
       </c>
@@ -1036,31 +995,28 @@
         <v>3464.6239999999998</v>
       </c>
       <c r="E14" t="n">
-        <v>20411209</v>
+        <v>3652.5</v>
       </c>
       <c r="F14" t="n">
-        <v>3652.5</v>
+        <v>11.2153729999999996</v>
       </c>
       <c r="G14" t="n">
-        <v>11.2153729999999996</v>
+        <v>47.5438290000000023</v>
       </c>
       <c r="H14" t="n">
-        <v>47.5438290000000023</v>
+        <v>838.467399999999998</v>
       </c>
       <c r="I14" t="n">
-        <v>838.467399999999998</v>
+        <v>1269.9081000000001</v>
       </c>
       <c r="J14" t="n">
-        <v>1269.9081000000001</v>
+        <v>2.93887300000000007</v>
       </c>
       <c r="K14" t="n">
-        <v>2.93887300000000007</v>
-      </c>
-      <c r="L14" t="n">
         <v>606.200000000000045</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:12">
       <c r="A15" t="n">
         <v>33357</v>
       </c>
@@ -1074,31 +1030,28 @@
         <v>5890.28169999999955</v>
       </c>
       <c r="E15" t="n">
-        <v>20420715</v>
+        <v>4017.75</v>
       </c>
       <c r="F15" t="n">
-        <v>4017.75</v>
+        <v>9.9130395999999994</v>
       </c>
       <c r="G15" t="n">
-        <v>9.9130395999999994</v>
+        <v>47.5500559999999979</v>
       </c>
       <c r="H15" t="n">
-        <v>47.5500559999999979</v>
+        <v>2204.45040000000017</v>
       </c>
       <c r="I15" t="n">
-        <v>2204.45040000000017</v>
+        <v>2388.80709999999999</v>
       </c>
       <c r="J15" t="n">
-        <v>2388.80709999999999</v>
+        <v>2.33973090000000017</v>
       </c>
       <c r="K15" t="n">
-        <v>2.33973090000000017</v>
-      </c>
-      <c r="L15" t="n">
         <v>547</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:12">
       <c r="A16" t="n">
         <v>33357</v>
       </c>
@@ -1112,36 +1065,33 @@
         <v>5752.79929999999968</v>
       </c>
       <c r="E16" t="n">
-        <v>20410808</v>
+        <v>3652.5</v>
       </c>
       <c r="F16" t="n">
-        <v>3652.5</v>
+        <v>12.0570850000000007</v>
       </c>
       <c r="G16" t="n">
-        <v>12.0570850000000007</v>
+        <v>47.585517000000003</v>
       </c>
       <c r="H16" t="n">
-        <v>47.585517000000003</v>
+        <v>1548.11470000000008</v>
       </c>
       <c r="I16" t="n">
-        <v>1548.11470000000008</v>
+        <v>2889.26580000000013</v>
       </c>
       <c r="J16" t="n">
-        <v>2889.26580000000013</v>
+        <v>3.35616469999999989</v>
       </c>
       <c r="K16" t="n">
-        <v>3.35616469999999989</v>
-      </c>
-      <c r="L16" t="n">
         <v>565.399999999999977</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:12">
       <c r="A17" t="n">
         <v>33357</v>
       </c>
       <c r="B17" t="n">
-        <v>1.67153029999999987</v>
+        <v>1.67153029999999969</v>
       </c>
       <c r="C17" t="n">
         <v>22.378544999999999</v>
@@ -1150,31 +1100,28 @@
         <v>5859.94200000000001</v>
       </c>
       <c r="E17" t="n">
-        <v>20420429</v>
+        <v>4017.75</v>
       </c>
       <c r="F17" t="n">
-        <v>4017.75</v>
+        <v>10.3595109999999995</v>
       </c>
       <c r="G17" t="n">
-        <v>10.3595109999999995</v>
+        <v>47.5706599999999966</v>
       </c>
       <c r="H17" t="n">
-        <v>47.5706599999999966</v>
+        <v>2054.71079999999984</v>
       </c>
       <c r="I17" t="n">
-        <v>2054.71079999999984</v>
+        <v>2502.11229999999978</v>
       </c>
       <c r="J17" t="n">
-        <v>2502.11229999999978</v>
+        <v>2.53854390000000008</v>
       </c>
       <c r="K17" t="n">
-        <v>2.53854390000000008</v>
-      </c>
-      <c r="L17" t="n">
         <v>553.100000000000023</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:12">
       <c r="A18" t="n">
         <v>33357</v>
       </c>
@@ -1188,31 +1135,28 @@
         <v>5714.38550000000032</v>
       </c>
       <c r="E18" t="n">
-        <v>20410526</v>
+        <v>3652.5</v>
       </c>
       <c r="F18" t="n">
-        <v>3652.5</v>
+        <v>12.6267200000000006</v>
       </c>
       <c r="G18" t="n">
-        <v>12.6267200000000006</v>
+        <v>47.6547180000000026</v>
       </c>
       <c r="H18" t="n">
-        <v>47.6547180000000026</v>
+        <v>1388.7047</v>
       </c>
       <c r="I18" t="n">
-        <v>1388.7047</v>
+        <v>2977.8476999999998</v>
       </c>
       <c r="J18" t="n">
-        <v>2977.8476999999998</v>
+        <v>3.65121930000000017</v>
       </c>
       <c r="K18" t="n">
-        <v>3.65121930000000017</v>
-      </c>
-      <c r="L18" t="n">
         <v>597.799999999999955</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:12">
       <c r="A19" t="n">
         <v>33357</v>
       </c>
@@ -1226,31 +1170,28 @@
         <v>4516.58790000000045</v>
       </c>
       <c r="E19" t="n">
-        <v>20420706</v>
+        <v>4017.75</v>
       </c>
       <c r="F19" t="n">
-        <v>4017.75</v>
+        <v>10.6902080000000002</v>
       </c>
       <c r="G19" t="n">
-        <v>10.6902080000000002</v>
+        <v>50.8122940000000014</v>
       </c>
       <c r="H19" t="n">
-        <v>50.8122940000000014</v>
+        <v>1427.52450000000022</v>
       </c>
       <c r="I19" t="n">
-        <v>1427.52449999999999</v>
+        <v>1892.72849999999994</v>
       </c>
       <c r="J19" t="n">
-        <v>1892.72849999999994</v>
+        <v>2.69028009999999984</v>
       </c>
       <c r="K19" t="n">
-        <v>2.69028009999999984</v>
-      </c>
-      <c r="L19" t="n">
         <v>446.399999999999977</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:12">
       <c r="A20" t="n">
         <v>33357</v>
       </c>
@@ -1264,31 +1205,28 @@
         <v>5803.71230000000014</v>
       </c>
       <c r="E20" t="n">
-        <v>20410801</v>
+        <v>3652.5</v>
       </c>
       <c r="F20" t="n">
-        <v>3652.5</v>
+        <v>12.1097660000000005</v>
       </c>
       <c r="G20" t="n">
-        <v>12.1097660000000005</v>
+        <v>47.588994999999997</v>
       </c>
       <c r="H20" t="n">
-        <v>47.588994999999997</v>
+        <v>1537.42020000000002</v>
       </c>
       <c r="I20" t="n">
-        <v>1537.42020000000002</v>
+        <v>2906.61099999999988</v>
       </c>
       <c r="J20" t="n">
-        <v>2906.61099999999988</v>
+        <v>3.38303170000000009</v>
       </c>
       <c r="K20" t="n">
-        <v>3.38303170000000009</v>
-      </c>
-      <c r="L20" t="n">
         <v>609.700000000000045</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:12">
       <c r="A21" t="n">
         <v>33357</v>
       </c>
@@ -1302,31 +1240,28 @@
         <v>5891.05689999999959</v>
       </c>
       <c r="E21" t="n">
-        <v>20420715</v>
+        <v>4017.75</v>
       </c>
       <c r="F21" t="n">
-        <v>4017.75</v>
+        <v>9.91239610000000049</v>
       </c>
       <c r="G21" t="n">
-        <v>9.91239610000000049</v>
+        <v>47.5502099999999999</v>
       </c>
       <c r="H21" t="n">
-        <v>47.5502099999999999</v>
+        <v>2204.51629999999977</v>
       </c>
       <c r="I21" t="n">
-        <v>2204.51629999999977</v>
+        <v>2388.47290000000021</v>
       </c>
       <c r="J21" t="n">
-        <v>2388.47290000000021</v>
+        <v>2.33944950000000018</v>
       </c>
       <c r="K21" t="n">
-        <v>2.33944950000000018</v>
-      </c>
-      <c r="L21" t="n">
         <v>548.100000000000023</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:12">
       <c r="A22" t="n">
         <v>33357</v>
       </c>
@@ -1340,31 +1275,28 @@
         <v>5756.0027</v>
       </c>
       <c r="E22" t="n">
-        <v>20410808</v>
+        <v>3652.5</v>
       </c>
       <c r="F22" t="n">
-        <v>3652.5</v>
+        <v>12.0545139999999993</v>
       </c>
       <c r="G22" t="n">
-        <v>12.0545139999999993</v>
+        <v>47.5853660000000005</v>
       </c>
       <c r="H22" t="n">
-        <v>47.5853660000000005</v>
+        <v>1548.50549999999998</v>
       </c>
       <c r="I22" t="n">
-        <v>1548.50549999999998</v>
+        <v>2888.17270000000008</v>
       </c>
       <c r="J22" t="n">
-        <v>2888.17270000000008</v>
+        <v>3.3548559</v>
       </c>
       <c r="K22" t="n">
-        <v>3.3548559</v>
-      </c>
-      <c r="L22" t="n">
         <v>569.299999999999955</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:12">
       <c r="A23" t="n">
         <v>33357</v>
       </c>
@@ -1378,31 +1310,28 @@
         <v>3781.93209999999999</v>
       </c>
       <c r="E23" t="n">
-        <v>20420822</v>
+        <v>4017.75</v>
       </c>
       <c r="F23" t="n">
-        <v>4017.75</v>
+        <v>9.71149559999999923</v>
       </c>
       <c r="G23" t="n">
-        <v>9.71149559999999923</v>
+        <v>47.5957739999999987</v>
       </c>
       <c r="H23" t="n">
-        <v>47.5957739999999987</v>
+        <v>1141.28839999999991</v>
       </c>
       <c r="I23" t="n">
-        <v>1141.28839999999991</v>
+        <v>1172.38779999999997</v>
       </c>
       <c r="J23" t="n">
-        <v>1172.38779999999997</v>
+        <v>2.25230269999999999</v>
       </c>
       <c r="K23" t="n">
-        <v>2.25230269999999999</v>
-      </c>
-      <c r="L23" t="n">
         <v>718.299999999999955</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:12">
       <c r="A24" t="n">
         <v>33357</v>
       </c>
@@ -1416,31 +1345,28 @@
         <v>3737.77640000000019</v>
       </c>
       <c r="E24" t="n">
-        <v>20410827</v>
+        <v>3652.5</v>
       </c>
       <c r="F24" t="n">
-        <v>3652.5</v>
+        <v>11.9319070000000007</v>
       </c>
       <c r="G24" t="n">
-        <v>11.9319070000000007</v>
+        <v>47.6028149999999997</v>
       </c>
       <c r="H24" t="n">
-        <v>47.6028149999999997</v>
+        <v>811.717499999999859</v>
       </c>
       <c r="I24" t="n">
-        <v>811.717499999999859</v>
+        <v>1469.02839999999992</v>
       </c>
       <c r="J24" t="n">
-        <v>1469.02839999999992</v>
+        <v>3.29267369999999993</v>
       </c>
       <c r="K24" t="n">
-        <v>3.29267369999999993</v>
-      </c>
-      <c r="L24" t="n">
         <v>707</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:12">
       <c r="A25" t="n">
         <v>33357</v>
       </c>
@@ -1454,31 +1380,28 @@
         <v>5735.32170000000042</v>
       </c>
       <c r="E25" t="n">
-        <v>20430825</v>
+        <v>4017.75</v>
       </c>
       <c r="F25" t="n">
-        <v>4017.75</v>
+        <v>9.60536710000000049</v>
       </c>
       <c r="G25" t="n">
-        <v>9.60536710000000049</v>
+        <v>57.2897260000000017</v>
       </c>
       <c r="H25" t="n">
-        <v>57.2897260000000017</v>
+        <v>2077.95600000000013</v>
       </c>
       <c r="I25" t="n">
-        <v>2077.95600000000013</v>
+        <v>2074.93379999999979</v>
       </c>
       <c r="J25" t="n">
-        <v>2074.93379999999979</v>
+        <v>2.20685330000000013</v>
       </c>
       <c r="K25" t="n">
-        <v>2.20685330000000013</v>
-      </c>
-      <c r="L25" t="n">
-        <v>832.399999999999977</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18">
+        <v>832.399999999999864</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" t="n">
         <v>33357</v>
       </c>
@@ -1492,31 +1415,28 @@
         <v>5910.92969999999968</v>
       </c>
       <c r="E26" t="n">
-        <v>20430521</v>
+        <v>4017.75</v>
       </c>
       <c r="F26" t="n">
-        <v>4017.75</v>
+        <v>8.92961539999999765</v>
       </c>
       <c r="G26" t="n">
-        <v>8.92961539999999765</v>
+        <v>51.5942989999999995</v>
       </c>
       <c r="H26" t="n">
-        <v>51.5942989999999995</v>
+        <v>2458.64150000000018</v>
       </c>
       <c r="I26" t="n">
-        <v>2458.64150000000018</v>
+        <v>2042.23710000000005</v>
       </c>
       <c r="J26" t="n">
-        <v>2042.23710000000005</v>
+        <v>1.92716059999999985</v>
       </c>
       <c r="K26" t="n">
-        <v>1.92716059999999985</v>
-      </c>
-      <c r="L26" t="n">
         <v>660.100000000000023</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:12">
       <c r="A27" t="n">
         <v>33357</v>
       </c>
@@ -1530,31 +1450,28 @@
         <v>5821.62060000000019</v>
       </c>
       <c r="E27" t="n">
-        <v>20420616</v>
+        <v>3652.5</v>
       </c>
       <c r="F27" t="n">
-        <v>3652.5</v>
+        <v>10.8142020000000016</v>
       </c>
       <c r="G27" t="n">
-        <v>10.8142019999999999</v>
+        <v>50.765036000000002</v>
       </c>
       <c r="H27" t="n">
-        <v>50.765036000000002</v>
+        <v>1839.87010000000009</v>
       </c>
       <c r="I27" t="n">
-        <v>1839.87010000000009</v>
+        <v>2517.84310000000005</v>
       </c>
       <c r="J27" t="n">
-        <v>2517.84310000000005</v>
+        <v>2.74813760000000018</v>
       </c>
       <c r="K27" t="n">
-        <v>2.74813760000000018</v>
-      </c>
-      <c r="L27" t="n">
         <v>713.899999999999977</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:12">
       <c r="A28" t="n">
         <v>33357</v>
       </c>
@@ -1568,31 +1485,28 @@
         <v>5925.09299999999985</v>
       </c>
       <c r="E28" t="n">
-        <v>20430803</v>
+        <v>4017.75</v>
       </c>
       <c r="F28" t="n">
-        <v>4017.75</v>
+        <v>8.56176540000000053</v>
       </c>
       <c r="G28" t="n">
-        <v>8.56176540000000053</v>
+        <v>51.6732620000000011</v>
       </c>
       <c r="H28" t="n">
-        <v>51.6732620000000011</v>
+        <v>2610.01099999999997</v>
       </c>
       <c r="I28" t="n">
-        <v>2610.01099999999997</v>
+        <v>1955.38609999999994</v>
       </c>
       <c r="J28" t="n">
-        <v>1955.38609999999994</v>
+        <v>1.78210460000000008</v>
       </c>
       <c r="K28" t="n">
-        <v>1.78210460000000008</v>
-      </c>
-      <c r="L28" t="n">
         <v>609.700000000000045</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:12">
       <c r="A29" t="n">
         <v>33357</v>
       </c>
@@ -1606,31 +1520,28 @@
         <v>5826.67699999999968</v>
       </c>
       <c r="E29" t="n">
-        <v>20420617</v>
+        <v>3652.5</v>
       </c>
       <c r="F29" t="n">
-        <v>3652.5</v>
+        <v>10.8086079999999995</v>
       </c>
       <c r="G29" t="n">
-        <v>10.8086079999999995</v>
+        <v>50.7668379999999999</v>
       </c>
       <c r="H29" t="n">
-        <v>50.7668379999999999</v>
+        <v>1840.47880000000009</v>
       </c>
       <c r="I29" t="n">
-        <v>1840.47880000000009</v>
+        <v>2515.09220000000005</v>
       </c>
       <c r="J29" t="n">
-        <v>2515.09220000000005</v>
+        <v>2.74551619999999996</v>
       </c>
       <c r="K29" t="n">
-        <v>2.74551619999999996</v>
-      </c>
-      <c r="L29" t="n">
         <v>721.100000000000023</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:12">
       <c r="A30" t="n">
         <v>33357</v>
       </c>
@@ -1644,31 +1555,28 @@
         <v>5456.39599999999973</v>
       </c>
       <c r="E30" t="n">
-        <v>20430530</v>
+        <v>4017.75</v>
       </c>
       <c r="F30" t="n">
-        <v>4017.75</v>
+        <v>10.2027970000000003</v>
       </c>
       <c r="G30" t="n">
-        <v>10.2027970000000003</v>
+        <v>57.3377359999999996</v>
       </c>
       <c r="H30" t="n">
-        <v>57.3377359999999996</v>
+        <v>1685.42669999999998</v>
       </c>
       <c r="I30" t="n">
-        <v>1685.42669999999998</v>
+        <v>1970.55030000000011</v>
       </c>
       <c r="J30" t="n">
-        <v>1970.55030000000011</v>
+        <v>2.46796119999999997</v>
       </c>
       <c r="K30" t="n">
-        <v>2.46796119999999997</v>
-      </c>
-      <c r="L30" t="n">
         <v>1050.40000000000009</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:12">
       <c r="A31" t="n">
         <v>33357</v>
       </c>
@@ -1682,31 +1590,28 @@
         <v>5925.63990000000013</v>
       </c>
       <c r="E31" t="n">
-        <v>20430803</v>
+        <v>4017.75</v>
       </c>
       <c r="F31" t="n">
-        <v>4017.75</v>
+        <v>8.56189370000000061</v>
       </c>
       <c r="G31" t="n">
-        <v>8.56189370000000061</v>
+        <v>51.6709109999999967</v>
       </c>
       <c r="H31" t="n">
-        <v>51.6709109999999967</v>
+        <v>2610.0324999999998</v>
       </c>
       <c r="I31" t="n">
-        <v>2610.0324999999998</v>
+        <v>1955.47340000000008</v>
       </c>
       <c r="J31" t="n">
-        <v>1955.47340000000008</v>
+        <v>1.78215430000000001</v>
       </c>
       <c r="K31" t="n">
-        <v>1.78215430000000001</v>
-      </c>
-      <c r="L31" t="n">
         <v>610.100000000000023</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:12">
       <c r="A32" t="n">
         <v>33367</v>
       </c>
@@ -1720,31 +1625,28 @@
         <v>5487.91749999999956</v>
       </c>
       <c r="E32" t="n">
-        <v>20360501</v>
+        <v>4017.75</v>
       </c>
       <c r="F32" t="n">
-        <v>4017.75</v>
+        <v>10.8633369999999996</v>
       </c>
       <c r="G32" t="n">
-        <v>10.8633369999999996</v>
+        <v>75.815566000000004</v>
       </c>
       <c r="H32" t="n">
-        <v>75.815566000000004</v>
+        <v>1629.62760000000003</v>
       </c>
       <c r="I32" t="n">
-        <v>1629.62760000000003</v>
+        <v>2258.17009999999982</v>
       </c>
       <c r="J32" t="n">
-        <v>2258.17009999999982</v>
+        <v>2.77120899999999981</v>
       </c>
       <c r="K32" t="n">
-        <v>2.77120899999999981</v>
-      </c>
-      <c r="L32" t="n">
         <v>850.200000000000045</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:12">
       <c r="A33" t="n">
         <v>33257</v>
       </c>
@@ -1758,31 +1660,28 @@
         <v>4304.59169999999995</v>
       </c>
       <c r="E33" t="n">
-        <v>20410430</v>
+        <v>4017.75</v>
       </c>
       <c r="F33" t="n">
-        <v>4017.75</v>
+        <v>12.4846780000000006</v>
       </c>
       <c r="G33" t="n">
-        <v>12.4846780000000006</v>
+        <v>47.3164969999999983</v>
       </c>
       <c r="H33" t="n">
-        <v>47.3164969999999983</v>
+        <v>971.095900000000029</v>
       </c>
       <c r="I33" t="n">
-        <v>971.095900000000029</v>
+        <v>2011.80439999999999</v>
       </c>
       <c r="J33" t="n">
-        <v>2011.80439999999999</v>
+        <v>3.57671569999999983</v>
       </c>
       <c r="K33" t="n">
-        <v>3.57671569999999983</v>
-      </c>
-      <c r="L33" t="n">
         <v>571.700000000000045</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:12">
       <c r="A34" t="n">
         <v>33257</v>
       </c>
@@ -1796,31 +1695,28 @@
         <v>4429.58929999999964</v>
       </c>
       <c r="E34" t="n">
-        <v>20410411</v>
+        <v>4017.75</v>
       </c>
       <c r="F34" t="n">
-        <v>4017.75</v>
+        <v>12.6220409999999994</v>
       </c>
       <c r="G34" t="n">
-        <v>12.6220409999999994</v>
+        <v>47.3468790000000013</v>
       </c>
       <c r="H34" t="n">
-        <v>47.3468790000000013</v>
+        <v>996.258600000000001</v>
       </c>
       <c r="I34" t="n">
-        <v>996.258600000000001</v>
+        <v>2133.89089999999987</v>
       </c>
       <c r="J34" t="n">
-        <v>2133.89089999999987</v>
+        <v>3.64875509999999981</v>
       </c>
       <c r="K34" t="n">
-        <v>3.64875509999999981</v>
-      </c>
-      <c r="L34" t="n">
         <v>549.399999999999977</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:12">
       <c r="A35" t="n">
         <v>33257</v>
       </c>
@@ -1834,31 +1730,28 @@
         <v>4430.5637999999999</v>
       </c>
       <c r="E35" t="n">
-        <v>20410701</v>
+        <v>4017.75</v>
       </c>
       <c r="F35" t="n">
-        <v>4017.75</v>
+        <v>12.4461300000000001</v>
       </c>
       <c r="G35" t="n">
-        <v>12.4461300000000001</v>
+        <v>47.8057289999999995</v>
       </c>
       <c r="H35" t="n">
-        <v>47.8057289999999995</v>
+        <v>1033.64319999999998</v>
       </c>
       <c r="I35" t="n">
-        <v>1033.64319999999998</v>
+        <v>2121.40920000000006</v>
       </c>
       <c r="J35" t="n">
-        <v>2121.40920000000006</v>
+        <v>3.55660260000000017</v>
       </c>
       <c r="K35" t="n">
-        <v>3.55660260000000017</v>
-      </c>
-      <c r="L35" t="n">
         <v>525.5</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:12">
       <c r="A36" t="n">
         <v>33257</v>
       </c>
@@ -1872,31 +1765,28 @@
         <v>4428.4983000000002</v>
       </c>
       <c r="E36" t="n">
-        <v>20410802</v>
+        <v>4017.75</v>
       </c>
       <c r="F36" t="n">
-        <v>4017.75</v>
+        <v>12.7385760000000001</v>
       </c>
       <c r="G36" t="n">
-        <v>12.7385760000000001</v>
+        <v>49.0786549999999977</v>
       </c>
       <c r="H36" t="n">
-        <v>49.0786549999999977</v>
+        <v>979.384300000000053</v>
       </c>
       <c r="I36" t="n">
-        <v>979.384300000000053</v>
+        <v>2157.76240000000007</v>
       </c>
       <c r="J36" t="n">
-        <v>2157.76240000000007</v>
+        <v>3.71031749999999994</v>
       </c>
       <c r="K36" t="n">
-        <v>3.71031749999999994</v>
-      </c>
-      <c r="L36" t="n">
         <v>541.399999999999977</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:12">
       <c r="A37" t="n">
         <v>32337</v>
       </c>
@@ -1910,31 +1800,28 @@
         <v>4839.87079999999969</v>
       </c>
       <c r="E37" t="n">
-        <v>20451005</v>
+        <v>4017.75</v>
       </c>
       <c r="F37" t="n">
-        <v>4017.75</v>
+        <v>11.5958080000000017</v>
       </c>
       <c r="G37" t="n">
-        <v>11.5958079999999999</v>
+        <v>44.3661910000000006</v>
       </c>
       <c r="H37" t="n">
-        <v>44.3661910000000006</v>
+        <v>1334.9224999999999</v>
       </c>
       <c r="I37" t="n">
-        <v>1334.9224999999999</v>
+        <v>2223.30380000000014</v>
       </c>
       <c r="J37" t="n">
-        <v>2223.30380000000014</v>
+        <v>3.1246577000000002</v>
       </c>
       <c r="K37" t="n">
-        <v>3.1246577000000002</v>
-      </c>
-      <c r="L37" t="n">
         <v>531.600000000000023</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:12">
       <c r="A38" t="n">
         <v>32337</v>
       </c>
@@ -1948,31 +1835,28 @@
         <v>3850.10449999999992</v>
       </c>
       <c r="E38" t="n">
-        <v>20441116</v>
+        <v>4017.75</v>
       </c>
       <c r="F38" t="n">
-        <v>4017.75</v>
+        <v>11.3124769999999994</v>
       </c>
       <c r="G38" t="n">
-        <v>11.3124769999999994</v>
+        <v>49.1263300000000029</v>
       </c>
       <c r="H38" t="n">
-        <v>49.1263300000000029</v>
+        <v>1030.6422</v>
       </c>
       <c r="I38" t="n">
-        <v>1030.6422</v>
+        <v>1599.44550000000004</v>
       </c>
       <c r="J38" t="n">
-        <v>1599.44550000000004</v>
+        <v>2.98584449999999979</v>
       </c>
       <c r="K38" t="n">
-        <v>2.98584449999999979</v>
-      </c>
-      <c r="L38" t="n">
         <v>470</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:12">
       <c r="A39" t="n">
         <v>32337</v>
       </c>
@@ -1986,31 +1870,28 @@
         <v>5193.8131000000003</v>
       </c>
       <c r="E39" t="n">
-        <v>20470308</v>
+        <v>4017.75</v>
       </c>
       <c r="F39" t="n">
-        <v>4017.75</v>
+        <v>10.5796650000000003</v>
       </c>
       <c r="G39" t="n">
-        <v>10.5796650000000003</v>
+        <v>40.563087000000003</v>
       </c>
       <c r="H39" t="n">
-        <v>40.563087000000003</v>
+        <v>1765.11590000000001</v>
       </c>
       <c r="I39" t="n">
-        <v>1765.11590000000001</v>
+        <v>2274.98619999999983</v>
       </c>
       <c r="J39" t="n">
-        <v>2274.98619999999983</v>
+        <v>2.63914049999999989</v>
       </c>
       <c r="K39" t="n">
-        <v>2.63914049999999989</v>
-      </c>
-      <c r="L39" t="n">
         <v>403.699999999999989</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:12">
       <c r="A40" t="n">
         <v>32337</v>
       </c>
@@ -2024,31 +1905,28 @@
         <v>5482.94589999999971</v>
       </c>
       <c r="E40" t="n">
-        <v>20431119</v>
+        <v>4017.75</v>
       </c>
       <c r="F40" t="n">
-        <v>4017.75</v>
+        <v>11.3261780000000005</v>
       </c>
       <c r="G40" t="n">
-        <v>11.3261780000000005</v>
+        <v>53.7082759999999979</v>
       </c>
       <c r="H40" t="n">
-        <v>53.7082759999999979</v>
+        <v>1515.36760000000004</v>
       </c>
       <c r="I40" t="n">
-        <v>1515.36760000000004</v>
+        <v>2359.76670000000013</v>
       </c>
       <c r="J40" t="n">
-        <v>2359.76670000000013</v>
+        <v>2.99249669999999988</v>
       </c>
       <c r="K40" t="n">
-        <v>2.99249669999999988</v>
-      </c>
-      <c r="L40" t="n">
-        <v>857.799999999999955</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18">
+        <v>857.799999999999841</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" t="n">
         <v>32337</v>
       </c>
@@ -2062,31 +1940,28 @@
         <v>3902.61999999999989</v>
       </c>
       <c r="E41" t="n">
-        <v>20441111</v>
+        <v>4017.75</v>
       </c>
       <c r="F41" t="n">
-        <v>4017.75</v>
+        <v>9.29907350000000044</v>
       </c>
       <c r="G41" t="n">
-        <v>9.29907350000000044</v>
+        <v>55.2479900000000015</v>
       </c>
       <c r="H41" t="n">
-        <v>55.2479900000000015</v>
+        <v>1370.79389999999989</v>
       </c>
       <c r="I41" t="n">
-        <v>1370.79389999999989</v>
+        <v>1260.23880000000008</v>
       </c>
       <c r="J41" t="n">
-        <v>1260.23880000000008</v>
+        <v>2.07798579999999999</v>
       </c>
       <c r="K41" t="n">
-        <v>2.07798579999999999</v>
-      </c>
-      <c r="L41" t="n">
         <v>521.600000000000023</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:12">
       <c r="A42" t="n">
         <v>32337</v>
       </c>
@@ -2100,31 +1975,28 @@
         <v>3849.50599999999986</v>
       </c>
       <c r="E42" t="n">
-        <v>20431117</v>
+        <v>3652.5</v>
       </c>
       <c r="F42" t="n">
-        <v>3652.5</v>
+        <v>11.3353800000000007</v>
       </c>
       <c r="G42" t="n">
-        <v>11.3353800000000007</v>
+        <v>53.6134199999999979</v>
       </c>
       <c r="H42" t="n">
-        <v>53.6134199999999979</v>
+        <v>1007.36580000000004</v>
       </c>
       <c r="I42" t="n">
-        <v>1007.36580000000004</v>
+        <v>1572.31060000000002</v>
       </c>
       <c r="J42" t="n">
-        <v>1572.31060000000002</v>
+        <v>2.99696789999999993</v>
       </c>
       <c r="K42" t="n">
-        <v>2.99696789999999993</v>
-      </c>
-      <c r="L42" t="n">
         <v>519.799999999999955</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:12">
       <c r="A43" t="n">
         <v>32337</v>
       </c>
@@ -2132,37 +2004,34 @@
         <v>15.2561149999999994</v>
       </c>
       <c r="C43" t="n">
-        <v>7.86247239999999881</v>
+        <v>7.86247239999999969</v>
       </c>
       <c r="D43" t="n">
         <v>4488.04429999999957</v>
       </c>
       <c r="E43" t="n">
-        <v>20440610</v>
+        <v>4017.75</v>
       </c>
       <c r="F43" t="n">
-        <v>4017.75</v>
+        <v>12.4625249999999994</v>
       </c>
       <c r="G43" t="n">
-        <v>12.4625249999999994</v>
+        <v>48.6357280000000003</v>
       </c>
       <c r="H43" t="n">
-        <v>48.6357280000000003</v>
+        <v>1018.73249999999996</v>
       </c>
       <c r="I43" t="n">
-        <v>1018.73249999999996</v>
+        <v>2099.1592999999998</v>
       </c>
       <c r="J43" t="n">
-        <v>2099.1592999999998</v>
+        <v>3.56515169999999992</v>
       </c>
       <c r="K43" t="n">
-        <v>3.56515169999999992</v>
-      </c>
-      <c r="L43" t="n">
         <v>620.200000000000045</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:12">
       <c r="A44" t="n">
         <v>32357</v>
       </c>
@@ -2176,31 +2045,28 @@
         <v>5159.47090000000026</v>
       </c>
       <c r="E44" t="n">
-        <v>20401110</v>
+        <v>4017.75</v>
       </c>
       <c r="F44" t="n">
-        <v>4017.75</v>
+        <v>13.1581930000000007</v>
       </c>
       <c r="G44" t="n">
-        <v>13.1581930000000007</v>
+        <v>48.0952270000000013</v>
       </c>
       <c r="H44" t="n">
-        <v>48.0952270000000013</v>
+        <v>1149.25669999999991</v>
       </c>
       <c r="I44" t="n">
-        <v>1149.25669999999991</v>
+        <v>2801.31840000000011</v>
       </c>
       <c r="J44" t="n">
-        <v>2801.31840000000011</v>
+        <v>3.93533400000000011</v>
       </c>
       <c r="K44" t="n">
-        <v>3.93533400000000011</v>
-      </c>
-      <c r="L44" t="n">
         <v>458.899999999999977</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:12">
       <c r="A45" t="n">
         <v>32357</v>
       </c>
@@ -2214,31 +2080,28 @@
         <v>5331.30029999999988</v>
       </c>
       <c r="E45" t="n">
-        <v>20400730</v>
+        <v>4017.75</v>
       </c>
       <c r="F45" t="n">
-        <v>4017.75</v>
+        <v>14.004721</v>
       </c>
       <c r="G45" t="n">
-        <v>14.004721</v>
+        <v>48.4365889999999979</v>
       </c>
       <c r="H45" t="n">
-        <v>48.4365889999999979</v>
+        <v>984.34050000000002</v>
       </c>
       <c r="I45" t="n">
-        <v>984.34050000000002</v>
+        <v>2936.22989999999982</v>
       </c>
       <c r="J45" t="n">
-        <v>2936.22989999999982</v>
+        <v>4.40472230000000042</v>
       </c>
       <c r="K45" t="n">
-        <v>4.40472230000000042</v>
-      </c>
-      <c r="L45" t="n">
         <v>660.700000000000045</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:12">
       <c r="A46" t="n">
         <v>32357</v>
       </c>
@@ -2252,31 +2115,28 @@
         <v>5160.33759999999984</v>
       </c>
       <c r="E46" t="n">
-        <v>20401110</v>
+        <v>4017.75</v>
       </c>
       <c r="F46" t="n">
-        <v>4017.75</v>
+        <v>13.1575349999999993</v>
       </c>
       <c r="G46" t="n">
-        <v>13.1575349999999993</v>
+        <v>48.0951359999999966</v>
       </c>
       <c r="H46" t="n">
-        <v>48.0951359999999966</v>
+        <v>1149.49090000000001</v>
       </c>
       <c r="I46" t="n">
-        <v>1149.49090000000001</v>
+        <v>2801.44639999999981</v>
       </c>
       <c r="J46" t="n">
-        <v>2801.44639999999981</v>
+        <v>3.93497669999999999</v>
       </c>
       <c r="K46" t="n">
-        <v>3.93497669999999999</v>
-      </c>
-      <c r="L46" t="n">
         <v>459.399999999999977</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:12">
       <c r="A47" t="n">
         <v>32357</v>
       </c>
@@ -2290,31 +2150,28 @@
         <v>5496.25799999999981</v>
       </c>
       <c r="E47" t="n">
-        <v>20411205</v>
+        <v>4017.75</v>
       </c>
       <c r="F47" t="n">
-        <v>4017.75</v>
+        <v>10.7611290000000004</v>
       </c>
       <c r="G47" t="n">
-        <v>10.7611290000000004</v>
+        <v>46.8255330000000001</v>
       </c>
       <c r="H47" t="n">
-        <v>46.8255330000000001</v>
+        <v>1835.11380000000008</v>
       </c>
       <c r="I47" t="n">
-        <v>1835.11380000000008</v>
+        <v>2477.60600000000022</v>
       </c>
       <c r="J47" t="n">
-        <v>2477.60600000000022</v>
+        <v>2.72330899999999998</v>
       </c>
       <c r="K47" t="n">
-        <v>2.72330899999999998</v>
-      </c>
-      <c r="L47" t="n">
         <v>433.5</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:12">
       <c r="A48" t="n">
         <v>32357</v>
       </c>
@@ -2328,31 +2185,28 @@
         <v>3900.35800000000017</v>
       </c>
       <c r="E48" t="n">
-        <v>20400930</v>
+        <v>3652.5</v>
       </c>
       <c r="F48" t="n">
-        <v>3652.5</v>
+        <v>13.4431139999999996</v>
       </c>
       <c r="G48" t="n">
-        <v>13.4431139999999996</v>
+        <v>48.2841250000000031</v>
       </c>
       <c r="H48" t="n">
-        <v>48.2841250000000031</v>
+        <v>766.481400000000008</v>
       </c>
       <c r="I48" t="n">
-        <v>766.481400000000008</v>
+        <v>2000.22610000000009</v>
       </c>
       <c r="J48" t="n">
-        <v>2000.22610000000009</v>
+        <v>4.09104919999999961</v>
       </c>
       <c r="K48" t="n">
-        <v>4.09104919999999961</v>
-      </c>
-      <c r="L48" t="n">
         <v>383.699999999999989</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:12">
       <c r="A49" t="n">
         <v>32357</v>
       </c>
@@ -2366,31 +2220,28 @@
         <v>5164.57589999999982</v>
       </c>
       <c r="E49" t="n">
-        <v>20401110</v>
+        <v>4017.75</v>
       </c>
       <c r="F49" t="n">
-        <v>4017.75</v>
+        <v>13.1600789999999996</v>
       </c>
       <c r="G49" t="n">
-        <v>13.1600789999999996</v>
+        <v>48.0961449999999999</v>
       </c>
       <c r="H49" t="n">
-        <v>48.0961449999999999</v>
+        <v>1149.74090000000001</v>
       </c>
       <c r="I49" t="n">
-        <v>1149.74090000000001</v>
+        <v>2803.76729999999998</v>
       </c>
       <c r="J49" t="n">
-        <v>2803.76729999999998</v>
+        <v>3.93635689999999983</v>
       </c>
       <c r="K49" t="n">
-        <v>3.93635689999999983</v>
-      </c>
-      <c r="L49" t="n">
         <v>461.100000000000023</v>
       </c>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:12">
       <c r="A50" t="n">
         <v>32357</v>
       </c>
@@ -2404,31 +2255,28 @@
         <v>4558.84860000000026</v>
       </c>
       <c r="E50" t="n">
-        <v>20410413</v>
+        <v>4017.75</v>
       </c>
       <c r="F50" t="n">
-        <v>4017.75</v>
+        <v>12.1368670000000005</v>
       </c>
       <c r="G50" t="n">
-        <v>12.1368670000000005</v>
+        <v>47.4812900000000013</v>
       </c>
       <c r="H50" t="n">
-        <v>47.4812900000000013</v>
+        <v>1142.80130000000008</v>
       </c>
       <c r="I50" t="n">
-        <v>1142.80130000000008</v>
+        <v>2174.94509999999991</v>
       </c>
       <c r="J50" t="n">
-        <v>2174.94509999999991</v>
+        <v>3.39688670000000004</v>
       </c>
       <c r="K50" t="n">
-        <v>3.39688670000000004</v>
-      </c>
-      <c r="L50" t="n">
         <v>491.100000000000023</v>
       </c>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:12">
       <c r="A51" t="n">
         <v>32357</v>
       </c>
@@ -2442,31 +2290,28 @@
         <v>5655.73019999999997</v>
       </c>
       <c r="E51" t="n">
-        <v>20410909</v>
+        <v>4017.75</v>
       </c>
       <c r="F51" t="n">
-        <v>4017.75</v>
+        <v>11.253603</v>
       </c>
       <c r="G51" t="n">
-        <v>11.253603</v>
+        <v>47.0139840000000007</v>
       </c>
       <c r="H51" t="n">
-        <v>47.0139840000000007</v>
+        <v>1687.37910000000011</v>
       </c>
       <c r="I51" t="n">
-        <v>1687.37910000000011</v>
+        <v>2580.27590000000009</v>
       </c>
       <c r="J51" t="n">
-        <v>2580.27590000000009</v>
+        <v>2.95732870000000005</v>
       </c>
       <c r="K51" t="n">
-        <v>2.95732870000000005</v>
-      </c>
-      <c r="L51" t="n">
         <v>638.100000000000023</v>
       </c>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52" spans="1:12">
       <c r="A52" t="n">
         <v>32357</v>
       </c>
@@ -2480,31 +2325,28 @@
         <v>5501.21339999999964</v>
       </c>
       <c r="E52" t="n">
-        <v>20411205</v>
+        <v>4017.75</v>
       </c>
       <c r="F52" t="n">
-        <v>4017.75</v>
+        <v>10.7582240000000002</v>
       </c>
       <c r="G52" t="n">
-        <v>10.7582240000000002</v>
+        <v>46.8245819999999995</v>
       </c>
       <c r="H52" t="n">
-        <v>46.8245819999999995</v>
+        <v>1835.65840000000003</v>
       </c>
       <c r="I52" t="n">
-        <v>1835.65840000000003</v>
+        <v>2476.50619999999981</v>
       </c>
       <c r="J52" t="n">
-        <v>2476.50619999999981</v>
+        <v>2.72195300000000007</v>
       </c>
       <c r="K52" t="n">
-        <v>2.72195300000000007</v>
-      </c>
-      <c r="L52" t="n">
         <v>439</v>
       </c>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:12">
       <c r="A53" t="n">
         <v>32357</v>
       </c>
@@ -2518,31 +2360,28 @@
         <v>3869.42110000000002</v>
       </c>
       <c r="E53" t="n">
-        <v>20400729</v>
+        <v>3652.5</v>
       </c>
       <c r="F53" t="n">
-        <v>3652.5</v>
+        <v>13.9958950000000009</v>
       </c>
       <c r="G53" t="n">
-        <v>13.9958950000000009</v>
+        <v>48.4551960000000008</v>
       </c>
       <c r="H53" t="n">
-        <v>48.4551960000000008</v>
+        <v>673.365800000000036</v>
       </c>
       <c r="I53" t="n">
-        <v>673.365800000000036</v>
+        <v>2004.4085</v>
       </c>
       <c r="J53" t="n">
-        <v>2004.4085</v>
+        <v>4.39972470000000015</v>
       </c>
       <c r="K53" t="n">
-        <v>4.39972470000000015</v>
-      </c>
-      <c r="L53" t="n">
         <v>441.600000000000023</v>
       </c>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:12">
       <c r="A54" t="n">
         <v>32357</v>
       </c>
@@ -2556,31 +2395,28 @@
         <v>5493.62939999999981</v>
       </c>
       <c r="E54" t="n">
-        <v>20411204</v>
+        <v>4017.75</v>
       </c>
       <c r="F54" t="n">
-        <v>4017.75</v>
+        <v>10.7644000000000002</v>
       </c>
       <c r="G54" t="n">
-        <v>10.7644000000000002</v>
+        <v>46.8260560000000012</v>
       </c>
       <c r="H54" t="n">
-        <v>46.8260560000000012</v>
+        <v>1834.60750000000007</v>
       </c>
       <c r="I54" t="n">
-        <v>1834.60750000000007</v>
+        <v>2478.98930000000018</v>
       </c>
       <c r="J54" t="n">
-        <v>2478.98930000000018</v>
+        <v>2.72483649999999988</v>
       </c>
       <c r="K54" t="n">
-        <v>2.72483649999999988</v>
-      </c>
-      <c r="L54" t="n">
         <v>430</v>
       </c>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:12">
       <c r="A55" t="n">
         <v>32357</v>
       </c>
@@ -2594,31 +2430,28 @@
         <v>3903.06660000000011</v>
       </c>
       <c r="E55" t="n">
-        <v>20400930</v>
+        <v>3652.5</v>
       </c>
       <c r="F55" t="n">
-        <v>3652.5</v>
+        <v>13.4440419999999996</v>
       </c>
       <c r="G55" t="n">
-        <v>13.4440419999999996</v>
+        <v>48.2846990000000034</v>
       </c>
       <c r="H55" t="n">
-        <v>48.2846990000000034</v>
+        <v>766.792599999999993</v>
       </c>
       <c r="I55" t="n">
-        <v>766.792599999999993</v>
+        <v>2001.4822999999999</v>
       </c>
       <c r="J55" t="n">
-        <v>2001.4822999999999</v>
+        <v>4.09156049999999993</v>
       </c>
       <c r="K55" t="n">
-        <v>4.09156049999999993</v>
-      </c>
-      <c r="L55" t="n">
         <v>384.800000000000011</v>
       </c>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:12">
       <c r="A56" t="n">
         <v>32357</v>
       </c>
@@ -2632,31 +2465,28 @@
         <v>5346.77679999999964</v>
       </c>
       <c r="E56" t="n">
-        <v>20421227</v>
+        <v>4017.75</v>
       </c>
       <c r="F56" t="n">
-        <v>4017.75</v>
+        <v>9.67474290000000003</v>
       </c>
       <c r="G56" t="n">
-        <v>9.67474290000000003</v>
+        <v>51.2413480000000021</v>
       </c>
       <c r="H56" t="n">
-        <v>51.2413480000000021</v>
+        <v>1912.3592000000001</v>
       </c>
       <c r="I56" t="n">
-        <v>1912.3592000000001</v>
+        <v>1945.31600000000003</v>
       </c>
       <c r="J56" t="n">
-        <v>1945.31600000000003</v>
+        <v>2.23651720000000021</v>
       </c>
       <c r="K56" t="n">
-        <v>2.23651720000000021</v>
-      </c>
-      <c r="L56" t="n">
         <v>739.100000000000023</v>
       </c>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:12">
       <c r="A57" t="n">
         <v>32357</v>
       </c>
@@ -2670,31 +2500,28 @@
         <v>4453.48269999999957</v>
       </c>
       <c r="E57" t="n">
-        <v>20410917</v>
+        <v>3652.5</v>
       </c>
       <c r="F57" t="n">
-        <v>3652.5</v>
+        <v>11.7480420000000017</v>
       </c>
       <c r="G57" t="n">
-        <v>11.7480419999999999</v>
+        <v>47.5163989999999998</v>
       </c>
       <c r="H57" t="n">
-        <v>47.5163989999999998</v>
+        <v>1190.3735999999999</v>
       </c>
       <c r="I57" t="n">
-        <v>1190.3735999999999</v>
+        <v>2058.77759999999989</v>
       </c>
       <c r="J57" t="n">
-        <v>2058.77759999999989</v>
+        <v>3.2003134000000002</v>
       </c>
       <c r="K57" t="n">
-        <v>3.2003134000000002</v>
-      </c>
-      <c r="L57" t="n">
         <v>454.300000000000011</v>
       </c>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:12">
       <c r="A58" t="n">
         <v>32357</v>
       </c>
@@ -2708,31 +2535,28 @@
         <v>5403.00150000000031</v>
       </c>
       <c r="E58" t="n">
-        <v>20420215</v>
+        <v>4017.75</v>
       </c>
       <c r="F58" t="n">
-        <v>4017.75</v>
+        <v>10.3425940000000001</v>
       </c>
       <c r="G58" t="n">
-        <v>10.3425940000000001</v>
+        <v>46.6930550000000011</v>
       </c>
       <c r="H58" t="n">
-        <v>46.6930550000000011</v>
+        <v>1936.31660000000011</v>
       </c>
       <c r="I58" t="n">
-        <v>1936.31660000000011</v>
+        <v>2347.62950000000001</v>
       </c>
       <c r="J58" t="n">
-        <v>2347.62950000000001</v>
+        <v>2.53088360000000012</v>
       </c>
       <c r="K58" t="n">
-        <v>2.53088360000000012</v>
-      </c>
-      <c r="L58" t="n">
         <v>369.100000000000023</v>
       </c>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:12">
       <c r="A59" t="n">
         <v>32357</v>
       </c>
@@ -2746,31 +2570,28 @@
         <v>5401.5006999999996</v>
       </c>
       <c r="E59" t="n">
-        <v>20420215</v>
+        <v>4017.75</v>
       </c>
       <c r="F59" t="n">
-        <v>4017.75</v>
+        <v>10.3435319999999997</v>
       </c>
       <c r="G59" t="n">
-        <v>10.3435319999999997</v>
+        <v>46.6933459999999982</v>
       </c>
       <c r="H59" t="n">
-        <v>46.6933459999999982</v>
+        <v>1936.08870000000002</v>
       </c>
       <c r="I59" t="n">
-        <v>1936.08870000000002</v>
+        <v>2347.92399999999998</v>
       </c>
       <c r="J59" t="n">
-        <v>2347.92399999999998</v>
+        <v>2.53130830000000007</v>
       </c>
       <c r="K59" t="n">
-        <v>2.53130830000000007</v>
-      </c>
-      <c r="L59" t="n">
         <v>367.5</v>
       </c>
     </row>
-    <row r="60" spans="1:18">
+    <row r="60" spans="1:12">
       <c r="A60" t="n">
         <v>32357</v>
       </c>
@@ -2784,31 +2605,28 @@
         <v>5078.74150000000009</v>
       </c>
       <c r="E60" t="n">
-        <v>20420623</v>
+        <v>4017.75</v>
       </c>
       <c r="F60" t="n">
-        <v>4017.75</v>
+        <v>9.69238430000000051</v>
       </c>
       <c r="G60" t="n">
-        <v>9.69238430000000051</v>
+        <v>46.532668000000001</v>
       </c>
       <c r="H60" t="n">
-        <v>46.532668000000001</v>
+        <v>2003.75070000000005</v>
       </c>
       <c r="I60" t="n">
-        <v>2003.75070000000005</v>
+        <v>2047.89550000000008</v>
       </c>
       <c r="J60" t="n">
-        <v>2047.89550000000008</v>
+        <v>2.2440882000000002</v>
       </c>
       <c r="K60" t="n">
-        <v>2.2440882000000002</v>
-      </c>
-      <c r="L60" t="n">
         <v>277.100000000000023</v>
       </c>
     </row>
-    <row r="61" spans="1:18">
+    <row r="61" spans="1:12">
       <c r="A61" t="n">
         <v>32357</v>
       </c>
@@ -2822,31 +2640,28 @@
         <v>5064.05050000000028</v>
       </c>
       <c r="E61" t="n">
-        <v>20410625</v>
+        <v>3652.5</v>
       </c>
       <c r="F61" t="n">
-        <v>3652.5</v>
+        <v>11.71523</v>
       </c>
       <c r="G61" t="n">
-        <v>11.71523</v>
+        <v>47.2179130000000029</v>
       </c>
       <c r="H61" t="n">
-        <v>47.2179130000000029</v>
+        <v>1486.79909999999995</v>
       </c>
       <c r="I61" t="n">
-        <v>1486.79909999999995</v>
+        <v>2550.66240000000016</v>
       </c>
       <c r="J61" t="n">
-        <v>2550.66240000000016</v>
+        <v>3.18394410000000017</v>
       </c>
       <c r="K61" t="n">
-        <v>3.18394410000000017</v>
-      </c>
-      <c r="L61" t="n">
         <v>276.600000000000023</v>
       </c>
     </row>
-    <row r="62" spans="1:18">
+    <row r="62" spans="1:12">
       <c r="A62" t="n">
         <v>32357</v>
       </c>
@@ -2860,31 +2675,28 @@
         <v>5065.31360000000041</v>
       </c>
       <c r="E62" t="n">
-        <v>20420624</v>
+        <v>4017.75</v>
       </c>
       <c r="F62" t="n">
-        <v>4017.75</v>
+        <v>9.69101610000000058</v>
       </c>
       <c r="G62" t="n">
-        <v>9.69101610000000058</v>
+        <v>46.5405110000000022</v>
       </c>
       <c r="H62" t="n">
-        <v>46.5405110000000022</v>
+        <v>2003.71370000000002</v>
       </c>
       <c r="I62" t="n">
-        <v>2003.71370000000002</v>
+        <v>2047.11079999999993</v>
       </c>
       <c r="J62" t="n">
-        <v>2047.11079999999993</v>
+        <v>2.24350059999999996</v>
       </c>
       <c r="K62" t="n">
-        <v>2.24350059999999996</v>
-      </c>
-      <c r="L62" t="n">
         <v>264.5</v>
       </c>
     </row>
-    <row r="63" spans="1:18">
+    <row r="63" spans="1:12">
       <c r="A63" t="n">
         <v>32357</v>
       </c>
@@ -2898,31 +2710,28 @@
         <v>5057.85159999999996</v>
       </c>
       <c r="E63" t="n">
-        <v>20410626</v>
+        <v>3652.5</v>
       </c>
       <c r="F63" t="n">
-        <v>3652.5</v>
+        <v>11.7102149999999998</v>
       </c>
       <c r="G63" t="n">
-        <v>11.7102149999999998</v>
+        <v>47.2134190000000018</v>
       </c>
       <c r="H63" t="n">
-        <v>47.2134190000000018</v>
+        <v>1486.24520000000007</v>
       </c>
       <c r="I63" t="n">
-        <v>1486.24520000000007</v>
+        <v>2546.54889999999978</v>
       </c>
       <c r="J63" t="n">
-        <v>2546.54889999999978</v>
+        <v>3.1814452000000002</v>
       </c>
       <c r="K63" t="n">
-        <v>3.1814452000000002</v>
-      </c>
-      <c r="L63" t="n">
         <v>275.100000000000023</v>
       </c>
     </row>
-    <row r="64" spans="1:18">
+    <row r="64" spans="1:12">
       <c r="A64" t="n">
         <v>32357</v>
       </c>
@@ -2936,31 +2745,28 @@
         <v>5076.79370000000017</v>
       </c>
       <c r="E64" t="n">
-        <v>20420623</v>
+        <v>4017.75</v>
       </c>
       <c r="F64" t="n">
-        <v>4017.75</v>
+        <v>9.69221789999999928</v>
       </c>
       <c r="G64" t="n">
-        <v>9.69221789999999928</v>
+        <v>46.5326260000000005</v>
       </c>
       <c r="H64" t="n">
-        <v>46.5326260000000005</v>
+        <v>2003.22510000000011</v>
       </c>
       <c r="I64" t="n">
-        <v>2003.22510000000011</v>
+        <v>2047.26749999999993</v>
       </c>
       <c r="J64" t="n">
-        <v>2047.26749999999993</v>
+        <v>2.24401669999999998</v>
       </c>
       <c r="K64" t="n">
-        <v>2.24401669999999998</v>
-      </c>
-      <c r="L64" t="n">
         <v>276.300000000000011</v>
       </c>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:12">
       <c r="A65" t="n">
         <v>32357</v>
       </c>
@@ -2974,31 +2780,28 @@
         <v>5066.41110000000026</v>
       </c>
       <c r="E65" t="n">
-        <v>20410624</v>
+        <v>3652.5</v>
       </c>
       <c r="F65" t="n">
-        <v>3652.5</v>
+        <v>11.7164450000000002</v>
       </c>
       <c r="G65" t="n">
-        <v>11.7164450000000002</v>
+        <v>47.2195549999999997</v>
       </c>
       <c r="H65" t="n">
-        <v>47.2195549999999997</v>
+        <v>1486.75759999999991</v>
       </c>
       <c r="I65" t="n">
-        <v>1486.75759999999991</v>
+        <v>2551.35789999999997</v>
       </c>
       <c r="J65" t="n">
-        <v>2551.35789999999997</v>
+        <v>3.18454939999999986</v>
       </c>
       <c r="K65" t="n">
-        <v>3.18454939999999986</v>
-      </c>
-      <c r="L65" t="n">
         <v>278.300000000000011</v>
       </c>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66" spans="1:12">
       <c r="A66" t="n">
         <v>32357</v>
       </c>
@@ -3012,31 +2815,28 @@
         <v>5481.78340000000026</v>
       </c>
       <c r="E66" t="n">
-        <v>20430330</v>
+        <v>4017.75</v>
       </c>
       <c r="F66" t="n">
-        <v>4017.75</v>
+        <v>9.13078439999999958</v>
       </c>
       <c r="G66" t="n">
-        <v>9.13078439999999958</v>
+        <v>51.1313249999999968</v>
       </c>
       <c r="H66" t="n">
-        <v>51.1313249999999968</v>
+        <v>2191.65079999999989</v>
       </c>
       <c r="I66" t="n">
-        <v>2191.65079999999989</v>
+        <v>1924.3732</v>
       </c>
       <c r="J66" t="n">
-        <v>1924.3732</v>
+        <v>2.00865289999999996</v>
       </c>
       <c r="K66" t="n">
-        <v>2.00865289999999996</v>
-      </c>
-      <c r="L66" t="n">
         <v>615.799999999999955</v>
       </c>
     </row>
-    <row r="67" spans="1:18">
+    <row r="67" spans="1:12">
       <c r="A67" t="n">
         <v>32357</v>
       </c>
@@ -3050,69 +2850,63 @@
         <v>5405.18469999999979</v>
       </c>
       <c r="E67" t="n">
-        <v>20420411</v>
+        <v>3652.5</v>
       </c>
       <c r="F67" t="n">
-        <v>3652.5</v>
+        <v>11.1745330000000003</v>
       </c>
       <c r="G67" t="n">
-        <v>11.1745330000000003</v>
+        <v>50.3638520000000014</v>
       </c>
       <c r="H67" t="n">
-        <v>50.3638520000000014</v>
+        <v>1614.39390000000003</v>
       </c>
       <c r="I67" t="n">
-        <v>1614.39390000000003</v>
+        <v>2420.1280999999999</v>
       </c>
       <c r="J67" t="n">
-        <v>2420.1280999999999</v>
+        <v>2.91921099999999978</v>
       </c>
       <c r="K67" t="n">
-        <v>2.91921099999999978</v>
-      </c>
-      <c r="L67" t="n">
         <v>620.700000000000045</v>
       </c>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:12">
       <c r="A68" t="n">
         <v>32357</v>
       </c>
       <c r="B68" t="n">
-        <v>9.58645340000000168</v>
+        <v>9.5864533999999999</v>
       </c>
       <c r="C68" t="n">
-        <v>7.33563619999999883</v>
+        <v>7.33563619999999972</v>
       </c>
       <c r="D68" t="n">
         <v>5022.22199999999975</v>
       </c>
       <c r="E68" t="n">
-        <v>20430226</v>
+        <v>4017.75</v>
       </c>
       <c r="F68" t="n">
-        <v>4017.75</v>
+        <v>9.35702960000000061</v>
       </c>
       <c r="G68" t="n">
-        <v>9.35702960000000061</v>
+        <v>51.4039229999999989</v>
       </c>
       <c r="H68" t="n">
-        <v>51.4039229999999989</v>
+        <v>1895.01019999999994</v>
       </c>
       <c r="I68" t="n">
-        <v>1895.01019999999994</v>
+        <v>1769.80690000000004</v>
       </c>
       <c r="J68" t="n">
-        <v>1769.80690000000004</v>
+        <v>2.10210570000000008</v>
       </c>
       <c r="K68" t="n">
-        <v>2.10210570000000008</v>
-      </c>
-      <c r="L68" t="n">
         <v>607.399999999999977</v>
       </c>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69" spans="1:12">
       <c r="A69" t="n">
         <v>32357</v>
       </c>
@@ -3126,31 +2920,28 @@
         <v>5027.84289999999964</v>
       </c>
       <c r="E69" t="n">
-        <v>20420307</v>
+        <v>3652.5</v>
       </c>
       <c r="F69" t="n">
-        <v>3652.5</v>
+        <v>11.4971549999999993</v>
       </c>
       <c r="G69" t="n">
-        <v>11.4971549999999993</v>
+        <v>50.6041990000000013</v>
       </c>
       <c r="H69" t="n">
-        <v>50.6041990000000013</v>
+        <v>1380.83380000000011</v>
       </c>
       <c r="I69" t="n">
-        <v>1380.83380000000011</v>
+        <v>2244.03670000000011</v>
       </c>
       <c r="J69" t="n">
-        <v>2244.03670000000011</v>
+        <v>3.07602829999999994</v>
       </c>
       <c r="K69" t="n">
-        <v>3.07602829999999994</v>
-      </c>
-      <c r="L69" t="n">
         <v>653</v>
       </c>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70" spans="1:12">
       <c r="A70" t="n">
         <v>32357</v>
       </c>
@@ -3164,31 +2955,28 @@
         <v>5480.51490000000013</v>
       </c>
       <c r="E70" t="n">
-        <v>20430330</v>
+        <v>4017.75</v>
       </c>
       <c r="F70" t="n">
-        <v>4017.75</v>
+        <v>9.13060570000000027</v>
       </c>
       <c r="G70" t="n">
-        <v>9.13060570000000027</v>
+        <v>51.1305970000000016</v>
       </c>
       <c r="H70" t="n">
-        <v>51.1305970000000016</v>
+        <v>2191.77019999999993</v>
       </c>
       <c r="I70" t="n">
-        <v>2191.77019999999993</v>
+        <v>1924.38359999999989</v>
       </c>
       <c r="J70" t="n">
-        <v>1924.38359999999989</v>
+        <v>2.00857980000000014</v>
       </c>
       <c r="K70" t="n">
-        <v>2.00857980000000014</v>
-      </c>
-      <c r="L70" t="n">
         <v>614.399999999999977</v>
       </c>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="1:12">
       <c r="A71" t="n">
         <v>32357</v>
       </c>
@@ -3202,31 +2990,28 @@
         <v>5278.30389999999989</v>
       </c>
       <c r="E71" t="n">
-        <v>20410425</v>
+        <v>3287.25</v>
       </c>
       <c r="F71" t="n">
-        <v>3287.25</v>
+        <v>13.9670530000000017</v>
       </c>
       <c r="G71" t="n">
-        <v>13.9670529999999999</v>
+        <v>49.8646049999999974</v>
       </c>
       <c r="H71" t="n">
-        <v>49.8646049999999974</v>
+        <v>983.303300000000036</v>
       </c>
       <c r="I71" t="n">
-        <v>983.303300000000036</v>
+        <v>2907.0326</v>
       </c>
       <c r="J71" t="n">
-        <v>2907.0326</v>
+        <v>4.3834086000000001</v>
       </c>
       <c r="K71" t="n">
-        <v>4.3834086000000001</v>
-      </c>
-      <c r="L71" t="n">
         <v>638</v>
       </c>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:12">
       <c r="A72" t="n">
         <v>32357</v>
       </c>
@@ -3240,31 +3025,28 @@
         <v>5410.21860000000015</v>
       </c>
       <c r="E72" t="n">
-        <v>20420411</v>
+        <v>3652.5</v>
       </c>
       <c r="F72" t="n">
-        <v>3652.5</v>
+        <v>11.1755759999999995</v>
       </c>
       <c r="G72" t="n">
-        <v>11.1755759999999995</v>
+        <v>50.3662690000000026</v>
       </c>
       <c r="H72" t="n">
-        <v>50.3662690000000026</v>
+        <v>1614.82279999999992</v>
       </c>
       <c r="I72" t="n">
-        <v>1614.82279999999992</v>
+        <v>2421.4058</v>
       </c>
       <c r="J72" t="n">
-        <v>2421.4058</v>
+        <v>2.91971230000000013</v>
       </c>
       <c r="K72" t="n">
-        <v>2.91971230000000013</v>
-      </c>
-      <c r="L72" t="n">
         <v>624</v>
       </c>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73" spans="1:12">
       <c r="A73" t="n">
         <v>32357</v>
       </c>
@@ -3278,31 +3060,28 @@
         <v>4031.61769999999979</v>
       </c>
       <c r="E73" t="n">
-        <v>20430731</v>
+        <v>4017.75</v>
       </c>
       <c r="F73" t="n">
-        <v>4017.75</v>
+        <v>8.60515889999999928</v>
       </c>
       <c r="G73" t="n">
-        <v>8.60515889999999928</v>
+        <v>51.8361590000000021</v>
       </c>
       <c r="H73" t="n">
-        <v>51.8361590000000021</v>
+        <v>1595.75250000000005</v>
       </c>
       <c r="I73" t="n">
-        <v>1595.75250000000005</v>
+        <v>1210.30670000000009</v>
       </c>
       <c r="J73" t="n">
-        <v>1210.30670000000009</v>
+        <v>1.7989474999999997</v>
       </c>
       <c r="K73" t="n">
-        <v>1.79894749999999988</v>
-      </c>
-      <c r="L73" t="n">
         <v>475.600000000000023</v>
       </c>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:12">
       <c r="A74" t="n">
         <v>32357</v>
       </c>
@@ -3310,37 +3089,34 @@
         <v>21.6563049999999997</v>
       </c>
       <c r="C74" t="n">
-        <v>-7.9059014999999988</v>
+        <v>-7.90590149999999969</v>
       </c>
       <c r="D74" t="n">
         <v>3942.32639999999992</v>
       </c>
       <c r="E74" t="n">
-        <v>20410826</v>
+        <v>3287.25</v>
       </c>
       <c r="F74" t="n">
-        <v>3287.25</v>
+        <v>12.9838059999999995</v>
       </c>
       <c r="G74" t="n">
-        <v>12.9838059999999995</v>
+        <v>50.2858639999999966</v>
       </c>
       <c r="H74" t="n">
-        <v>50.2858639999999966</v>
+        <v>806.651899999999841</v>
       </c>
       <c r="I74" t="n">
-        <v>806.651899999999841</v>
+        <v>1885.50890000000004</v>
       </c>
       <c r="J74" t="n">
-        <v>1885.50890000000004</v>
+        <v>3.84118959999999987</v>
       </c>
       <c r="K74" t="n">
-        <v>3.84118959999999987</v>
-      </c>
-      <c r="L74" t="n">
         <v>500.199999999999989</v>
       </c>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:12">
       <c r="A75" t="n">
         <v>32357</v>
       </c>
@@ -3354,31 +3130,28 @@
         <v>3995.76429999999982</v>
       </c>
       <c r="E75" t="n">
-        <v>20420805</v>
+        <v>3652.5</v>
       </c>
       <c r="F75" t="n">
-        <v>3652.5</v>
+        <v>10.5086999999999993</v>
       </c>
       <c r="G75" t="n">
-        <v>10.5086999999999993</v>
+        <v>50.9015739999999965</v>
       </c>
       <c r="H75" t="n">
-        <v>50.9015739999999965</v>
+        <v>1228.09079999999994</v>
       </c>
       <c r="I75" t="n">
-        <v>1228.09079999999994</v>
+        <v>1554.22319999999991</v>
       </c>
       <c r="J75" t="n">
-        <v>1554.22319999999991</v>
+        <v>2.60653120000000005</v>
       </c>
       <c r="K75" t="n">
-        <v>2.60653120000000005</v>
-      </c>
-      <c r="L75" t="n">
         <v>463.5</v>
       </c>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:12">
       <c r="A76" t="n">
         <v>32237</v>
       </c>
@@ -3392,31 +3165,28 @@
         <v>4176.21119999999974</v>
       </c>
       <c r="E76" t="n">
-        <v>20410922</v>
+        <v>4017.75</v>
       </c>
       <c r="F76" t="n">
-        <v>4017.75</v>
+        <v>9.66412659999999946</v>
       </c>
       <c r="G76" t="n">
-        <v>9.66412659999999946</v>
+        <v>68.646878000000001</v>
       </c>
       <c r="H76" t="n">
-        <v>68.646878000000001</v>
+        <v>1415.64720000000011</v>
       </c>
       <c r="I76" t="n">
-        <v>1415.64720000000011</v>
+        <v>1435.96939999999995</v>
       </c>
       <c r="J76" t="n">
-        <v>1435.96939999999995</v>
+        <v>2.2319665999999998</v>
       </c>
       <c r="K76" t="n">
-        <v>2.2319665999999998</v>
-      </c>
-      <c r="L76" t="n">
         <v>574.600000000000023</v>
       </c>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:12">
       <c r="A77" t="n">
         <v>32237</v>
       </c>
@@ -3430,31 +3200,28 @@
         <v>5746.0667999999996</v>
       </c>
       <c r="E77" t="n">
-        <v>20410730</v>
+        <v>4017.75</v>
       </c>
       <c r="F77" t="n">
-        <v>4017.75</v>
+        <v>9.93728909999999921</v>
       </c>
       <c r="G77" t="n">
-        <v>9.93728909999999921</v>
+        <v>68.4222529999999978</v>
       </c>
       <c r="H77" t="n">
-        <v>68.4222529999999978</v>
+        <v>2004.60519999999997</v>
       </c>
       <c r="I77" t="n">
-        <v>2004.60519999999997</v>
+        <v>2186.18640000000005</v>
       </c>
       <c r="J77" t="n">
-        <v>2186.18640000000005</v>
+        <v>2.3503482</v>
       </c>
       <c r="K77" t="n">
-        <v>2.3503482</v>
-      </c>
-      <c r="L77" t="n">
-        <v>805.299999999999955</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18">
+        <v>805.299999999999841</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78" t="n">
         <v>32237</v>
       </c>
@@ -3468,31 +3235,28 @@
         <v>5701.63550000000032</v>
       </c>
       <c r="E78" t="n">
-        <v>20430424</v>
+        <v>4017.75</v>
       </c>
       <c r="F78" t="n">
-        <v>4017.75</v>
+        <v>7.42707739999999994</v>
       </c>
       <c r="G78" t="n">
-        <v>7.42707739999999994</v>
+        <v>72.2424529999999834</v>
       </c>
       <c r="H78" t="n">
-        <v>72.2424529999999976</v>
+        <v>2790.17560000000003</v>
       </c>
       <c r="I78" t="n">
-        <v>2790.17560000000003</v>
+        <v>1495.53449999999998</v>
       </c>
       <c r="J78" t="n">
-        <v>1495.53449999999998</v>
+        <v>1.36787140000000007</v>
       </c>
       <c r="K78" t="n">
-        <v>1.36787140000000007</v>
-      </c>
-      <c r="L78" t="n">
         <v>665.899999999999977</v>
       </c>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79" spans="1:12">
       <c r="A79" t="n">
         <v>32237</v>
       </c>
@@ -3506,31 +3270,28 @@
         <v>5683.73390000000018</v>
       </c>
       <c r="E79" t="n">
-        <v>20420427</v>
+        <v>3652.5</v>
       </c>
       <c r="F79" t="n">
-        <v>3652.5</v>
+        <v>8.68493149999999758</v>
       </c>
       <c r="G79" t="n">
-        <v>8.68493149999999758</v>
+        <v>69.7345300000000066</v>
       </c>
       <c r="H79" t="n">
-        <v>69.7345300000000066</v>
+        <v>2371.4652000000001</v>
       </c>
       <c r="I79" t="n">
-        <v>2371.4652000000001</v>
+        <v>1839.6087</v>
       </c>
       <c r="J79" t="n">
-        <v>1839.6087</v>
+        <v>1.83009890000000013</v>
       </c>
       <c r="K79" t="n">
-        <v>1.83009890000000013</v>
-      </c>
-      <c r="L79" t="n">
         <v>722.700000000000045</v>
       </c>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80" spans="1:12">
       <c r="A80" t="n">
         <v>32237</v>
       </c>
@@ -3544,31 +3305,28 @@
         <v>4920.96849999999995</v>
       </c>
       <c r="E80" t="n">
-        <v>20420510</v>
+        <v>4017.75</v>
       </c>
       <c r="F80" t="n">
-        <v>4017.75</v>
+        <v>8.63570640000000012</v>
       </c>
       <c r="G80" t="n">
-        <v>8.63570640000000012</v>
+        <v>70.0500109999999978</v>
       </c>
       <c r="H80" t="n">
-        <v>70.0500109999999978</v>
+        <v>1975.46260000000007</v>
       </c>
       <c r="I80" t="n">
-        <v>1975.46260000000007</v>
+        <v>1511.29420000000005</v>
       </c>
       <c r="J80" t="n">
-        <v>1511.29420000000005</v>
+        <v>1.81084749999999985</v>
       </c>
       <c r="K80" t="n">
-        <v>1.81084749999999985</v>
-      </c>
-      <c r="L80" t="n">
         <v>684.200000000000045</v>
       </c>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:12">
       <c r="A81" t="n">
         <v>32237</v>
       </c>
@@ -3582,31 +3340,28 @@
         <v>4921.64559999999983</v>
       </c>
       <c r="E81" t="n">
-        <v>20420510</v>
+        <v>4017.75</v>
       </c>
       <c r="F81" t="n">
-        <v>4017.75</v>
+        <v>8.63584389999999757</v>
       </c>
       <c r="G81" t="n">
-        <v>8.63584389999999757</v>
+        <v>70.0496689999999944</v>
       </c>
       <c r="H81" t="n">
-        <v>70.0496689999999944</v>
+        <v>1976.09130000000005</v>
       </c>
       <c r="I81" t="n">
-        <v>1976.09130000000005</v>
+        <v>1511.83390000000009</v>
       </c>
       <c r="J81" t="n">
-        <v>1511.83390000000009</v>
+        <v>1.81090119999999999</v>
       </c>
       <c r="K81" t="n">
-        <v>1.81090119999999999</v>
-      </c>
-      <c r="L81" t="n">
         <v>683.700000000000045</v>
       </c>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:12">
       <c r="A82" t="n">
         <v>32237</v>
       </c>
@@ -3620,31 +3375,28 @@
         <v>5701.16209999999955</v>
       </c>
       <c r="E82" t="n">
-        <v>20430424</v>
+        <v>4017.75</v>
       </c>
       <c r="F82" t="n">
-        <v>4017.75</v>
+        <v>7.42573479999999986</v>
       </c>
       <c r="G82" t="n">
-        <v>7.42573479999999986</v>
+        <v>72.2510500000000064</v>
       </c>
       <c r="H82" t="n">
-        <v>72.2510500000000064</v>
+        <v>2793.17749999999978</v>
       </c>
       <c r="I82" t="n">
-        <v>2793.17749999999978</v>
+        <v>1496.52479999999991</v>
       </c>
       <c r="J82" t="n">
-        <v>1496.52479999999991</v>
+        <v>1.3674116999999999</v>
       </c>
       <c r="K82" t="n">
-        <v>1.3674116999999999</v>
-      </c>
-      <c r="L82" t="n">
         <v>661.5</v>
       </c>
     </row>
-    <row r="83" spans="1:18">
+    <row r="83" spans="1:12">
       <c r="A83" t="n">
         <v>32237</v>
       </c>
@@ -3658,31 +3410,28 @@
         <v>5679.98539999999957</v>
       </c>
       <c r="E83" t="n">
-        <v>20420428</v>
+        <v>3652.5</v>
       </c>
       <c r="F83" t="n">
-        <v>3652.5</v>
+        <v>8.68313039999999781</v>
       </c>
       <c r="G83" t="n">
-        <v>8.68313039999999781</v>
+        <v>69.7515999999999963</v>
       </c>
       <c r="H83" t="n">
-        <v>69.7515999999999963</v>
+        <v>2369.81629999999996</v>
       </c>
       <c r="I83" t="n">
-        <v>2369.81629999999996</v>
+        <v>1837.39750000000004</v>
       </c>
       <c r="J83" t="n">
-        <v>1837.39750000000004</v>
+        <v>1.82939279999999993</v>
       </c>
       <c r="K83" t="n">
-        <v>1.82939279999999993</v>
-      </c>
-      <c r="L83" t="n">
-        <v>722.799999999999955</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18">
+        <v>722.799999999999841</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
       <c r="A84" t="n">
         <v>32237</v>
       </c>
@@ -3696,31 +3445,28 @@
         <v>5700.10170000000016</v>
       </c>
       <c r="E84" t="n">
-        <v>20430424</v>
+        <v>4017.75</v>
       </c>
       <c r="F84" t="n">
-        <v>4017.75</v>
+        <v>7.42553450000000037</v>
       </c>
       <c r="G84" t="n">
-        <v>7.42553450000000037</v>
+        <v>72.2520219999999824</v>
       </c>
       <c r="H84" t="n">
-        <v>72.2520219999999824</v>
+        <v>2793.22659999999996</v>
       </c>
       <c r="I84" t="n">
-        <v>2793.22659999999996</v>
+        <v>1496.45880000000011</v>
       </c>
       <c r="J84" t="n">
-        <v>1496.45880000000011</v>
+        <v>1.36734310000000003</v>
       </c>
       <c r="K84" t="n">
-        <v>1.36734310000000003</v>
-      </c>
-      <c r="L84" t="n">
         <v>660.399999999999977</v>
       </c>
     </row>
-    <row r="85" spans="1:18">
+    <row r="85" spans="1:12">
       <c r="A85" t="n">
         <v>32237</v>
       </c>
@@ -3734,31 +3480,28 @@
         <v>5681.95430000000033</v>
       </c>
       <c r="E85" t="n">
-        <v>20420428</v>
+        <v>3652.5</v>
       </c>
       <c r="F85" t="n">
-        <v>3652.5</v>
+        <v>8.68178439999999796</v>
       </c>
       <c r="G85" t="n">
-        <v>8.68178439999999796</v>
+        <v>69.7582859999999982</v>
       </c>
       <c r="H85" t="n">
-        <v>69.7582859999999982</v>
+        <v>2370.40459999999985</v>
       </c>
       <c r="I85" t="n">
-        <v>2370.40459999999985</v>
+        <v>1837.1570999999999</v>
       </c>
       <c r="J85" t="n">
-        <v>1837.1570999999999</v>
+        <v>1.8288653</v>
       </c>
       <c r="K85" t="n">
-        <v>1.8288653</v>
-      </c>
-      <c r="L85" t="n">
-        <v>724.399999999999977</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18">
+        <v>724.399999999999864</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
       <c r="A86" t="n">
         <v>32257</v>
       </c>
@@ -3772,31 +3515,28 @@
         <v>4668.47819999999956</v>
       </c>
       <c r="E86" t="n">
-        <v>20401026</v>
+        <v>4017.75</v>
       </c>
       <c r="F86" t="n">
-        <v>4017.75</v>
+        <v>12.8139559999999992</v>
       </c>
       <c r="G86" t="n">
-        <v>12.8139559999999992</v>
+        <v>48.9660229999999999</v>
       </c>
       <c r="H86" t="n">
-        <v>48.9660229999999999</v>
+        <v>1036.57060000000001</v>
       </c>
       <c r="I86" t="n">
-        <v>1036.57060000000001</v>
+        <v>2325.72839999999997</v>
       </c>
       <c r="J86" t="n">
-        <v>2325.72839999999997</v>
+        <v>3.75035559999999979</v>
       </c>
       <c r="K86" t="n">
-        <v>3.75035559999999979</v>
-      </c>
-      <c r="L86" t="n">
         <v>556.200000000000045</v>
       </c>
     </row>
-    <row r="87" spans="1:18">
+    <row r="87" spans="1:12">
       <c r="A87" t="n">
         <v>32257</v>
       </c>
@@ -3810,31 +3550,28 @@
         <v>4049.37620000000015</v>
       </c>
       <c r="E87" t="n">
-        <v>20400809</v>
+        <v>4017.75</v>
       </c>
       <c r="F87" t="n">
-        <v>4017.75</v>
+        <v>13.8242639999999994</v>
       </c>
       <c r="G87" t="n">
-        <v>13.8242639999999994</v>
+        <v>48.5346529999999987</v>
       </c>
       <c r="H87" t="n">
-        <v>48.5346529999999987</v>
+        <v>724.905700000000024</v>
       </c>
       <c r="I87" t="n">
-        <v>724.905700000000024</v>
+        <v>2071.63029999999981</v>
       </c>
       <c r="J87" t="n">
-        <v>2071.63029999999981</v>
+        <v>4.30297109999999972</v>
       </c>
       <c r="K87" t="n">
-        <v>4.30297109999999972</v>
-      </c>
-      <c r="L87" t="n">
         <v>502.800000000000011</v>
       </c>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:12">
       <c r="A88" t="n">
         <v>32257</v>
       </c>
@@ -3848,31 +3585,28 @@
         <v>4036.49369999999999</v>
       </c>
       <c r="E88" t="n">
-        <v>20400808</v>
+        <v>4017.75</v>
       </c>
       <c r="F88" t="n">
-        <v>4017.75</v>
+        <v>13.753781</v>
       </c>
       <c r="G88" t="n">
-        <v>13.753781</v>
+        <v>48.6525600000000011</v>
       </c>
       <c r="H88" t="n">
-        <v>48.6525600000000011</v>
+        <v>725.829899999999839</v>
       </c>
       <c r="I88" t="n">
-        <v>725.829899999999839</v>
+        <v>2039.78559999999993</v>
       </c>
       <c r="J88" t="n">
-        <v>2039.78559999999993</v>
+        <v>4.26347450000000006</v>
       </c>
       <c r="K88" t="n">
-        <v>4.26347450000000006</v>
-      </c>
-      <c r="L88" t="n">
         <v>520.899999999999977</v>
       </c>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:12">
       <c r="A89" t="n">
         <v>32257</v>
       </c>
@@ -3886,31 +3620,28 @@
         <v>5255.89959999999974</v>
       </c>
       <c r="E89" t="n">
-        <v>20411215</v>
+        <v>4017.75</v>
       </c>
       <c r="F89" t="n">
-        <v>4017.75</v>
+        <v>10.9776399999999992</v>
       </c>
       <c r="G89" t="n">
-        <v>10.9776399999999992</v>
+        <v>47.0780829999999995</v>
       </c>
       <c r="H89" t="n">
-        <v>47.0780829999999995</v>
+        <v>1639.57449999999994</v>
       </c>
       <c r="I89" t="n">
-        <v>1639.57449999999994</v>
+        <v>2338.77250000000004</v>
       </c>
       <c r="J89" t="n">
-        <v>2338.77250000000004</v>
+        <v>2.82519419999999997</v>
       </c>
       <c r="K89" t="n">
-        <v>2.82519419999999997</v>
-      </c>
-      <c r="L89" t="n">
         <v>527.600000000000023</v>
       </c>
     </row>
-    <row r="90" spans="1:18">
+    <row r="90" spans="1:12">
       <c r="A90" t="n">
         <v>32257</v>
       </c>
@@ -3924,31 +3655,28 @@
         <v>5143.48790000000008</v>
       </c>
       <c r="E90" t="n">
-        <v>20401225</v>
+        <v>3652.5</v>
       </c>
       <c r="F90" t="n">
-        <v>3652.5</v>
+        <v>13.4262029999999992</v>
       </c>
       <c r="G90" t="n">
-        <v>13.4262029999999992</v>
+        <v>47.5414400000000015</v>
       </c>
       <c r="H90" t="n">
-        <v>47.5414400000000015</v>
+        <v>1075.0621000000001</v>
       </c>
       <c r="I90" t="n">
-        <v>1075.0621000000001</v>
+        <v>2794.18910000000005</v>
       </c>
       <c r="J90" t="n">
-        <v>2794.18910000000005</v>
+        <v>4.08174179999999964</v>
       </c>
       <c r="K90" t="n">
-        <v>4.08174179999999964</v>
-      </c>
-      <c r="L90" t="n">
         <v>524.200000000000045</v>
       </c>
     </row>
-    <row r="91" spans="1:18">
+    <row r="91" spans="1:12">
       <c r="A91" t="n">
         <v>32257</v>
       </c>
@@ -3962,31 +3690,28 @@
         <v>4799.30580000000009</v>
       </c>
       <c r="E91" t="n">
-        <v>20401122</v>
+        <v>4017.75</v>
       </c>
       <c r="F91" t="n">
-        <v>4017.75</v>
+        <v>13.676399</v>
       </c>
       <c r="G91" t="n">
-        <v>13.676399</v>
+        <v>47.6120299999999972</v>
       </c>
       <c r="H91" t="n">
-        <v>47.6120299999999972</v>
+        <v>891.892600000000016</v>
       </c>
       <c r="I91" t="n">
-        <v>891.892600000000016</v>
+        <v>2460.71379999999999</v>
       </c>
       <c r="J91" t="n">
-        <v>2460.71379999999999</v>
+        <v>4.22027199999999958</v>
       </c>
       <c r="K91" t="n">
-        <v>4.22027199999999958</v>
-      </c>
-      <c r="L91" t="n">
         <v>696.700000000000045</v>
       </c>
     </row>
-    <row r="92" spans="1:18">
+    <row r="92" spans="1:12">
       <c r="A92" t="n">
         <v>32257</v>
       </c>
@@ -4000,31 +3725,28 @@
         <v>4534.16579999999976</v>
       </c>
       <c r="E92" t="n">
-        <v>20410407</v>
+        <v>4017.75</v>
       </c>
       <c r="F92" t="n">
-        <v>4017.75</v>
+        <v>12.1625820000000004</v>
       </c>
       <c r="G92" t="n">
-        <v>12.1625820000000004</v>
+        <v>47.5110930000000025</v>
       </c>
       <c r="H92" t="n">
-        <v>47.5110930000000025</v>
+        <v>1065.30850000000009</v>
       </c>
       <c r="I92" t="n">
-        <v>1065.30850000000009</v>
+        <v>2040.2672</v>
       </c>
       <c r="J92" t="n">
-        <v>2040.2672</v>
+        <v>3.41005439999999993</v>
       </c>
       <c r="K92" t="n">
-        <v>3.41005439999999993</v>
-      </c>
-      <c r="L92" t="n">
         <v>678.600000000000023</v>
       </c>
     </row>
-    <row r="93" spans="1:18">
+    <row r="93" spans="1:12">
       <c r="A93" t="n">
         <v>32257</v>
       </c>
@@ -4038,31 +3760,28 @@
         <v>3993.79340000000002</v>
       </c>
       <c r="E93" t="n">
-        <v>20410522</v>
+        <v>4017.75</v>
       </c>
       <c r="F93" t="n">
-        <v>4017.75</v>
+        <v>12.3274700000000017</v>
       </c>
       <c r="G93" t="n">
-        <v>12.3274699999999999</v>
+        <v>47.2836250000000007</v>
       </c>
       <c r="H93" t="n">
-        <v>47.2836250000000007</v>
+        <v>923.422900000000027</v>
       </c>
       <c r="I93" t="n">
-        <v>923.422900000000027</v>
+        <v>1841.21810000000005</v>
       </c>
       <c r="J93" t="n">
-        <v>1841.21810000000005</v>
+        <v>3.49497340000000012</v>
       </c>
       <c r="K93" t="n">
-        <v>3.49497340000000012</v>
-      </c>
-      <c r="L93" t="n">
         <v>479.199999999999989</v>
       </c>
     </row>
-    <row r="94" spans="1:18">
+    <row r="94" spans="1:12">
       <c r="A94" t="n">
         <v>32257</v>
       </c>
@@ -4076,31 +3795,28 @@
         <v>5523.53629999999976</v>
       </c>
       <c r="E94" t="n">
-        <v>20411004</v>
+        <v>4017.75</v>
       </c>
       <c r="F94" t="n">
-        <v>4017.75</v>
+        <v>11.4244889999999995</v>
       </c>
       <c r="G94" t="n">
-        <v>11.4244889999999995</v>
+        <v>47.1316670000000002</v>
       </c>
       <c r="H94" t="n">
-        <v>47.1316670000000002</v>
+        <v>1611.63110000000006</v>
       </c>
       <c r="I94" t="n">
-        <v>1611.63110000000006</v>
+        <v>2572.09580000000005</v>
       </c>
       <c r="J94" t="n">
-        <v>2572.09580000000005</v>
+        <v>3.04041050000000013</v>
       </c>
       <c r="K94" t="n">
-        <v>3.04041050000000013</v>
-      </c>
-      <c r="L94" t="n">
         <v>589.799999999999955</v>
       </c>
     </row>
-    <row r="95" spans="1:18">
+    <row r="95" spans="1:12">
       <c r="A95" t="n">
         <v>32257</v>
       </c>
@@ -4108,37 +3824,34 @@
         <v>3.79963080000000009</v>
       </c>
       <c r="C95" t="n">
-        <v>-17.1082609999999988</v>
+        <v>-17.1082609999999953</v>
       </c>
       <c r="D95" t="n">
         <v>5623.25860000000011</v>
       </c>
       <c r="E95" t="n">
-        <v>20411109</v>
+        <v>4017.75</v>
       </c>
       <c r="F95" t="n">
-        <v>4017.75</v>
+        <v>11.1932200000000002</v>
       </c>
       <c r="G95" t="n">
-        <v>11.1932200000000002</v>
+        <v>47.0950580000000016</v>
       </c>
       <c r="H95" t="n">
-        <v>47.0950580000000016</v>
+        <v>1696.81999999999994</v>
       </c>
       <c r="I95" t="n">
-        <v>1696.81999999999994</v>
+        <v>2555.67079999999987</v>
       </c>
       <c r="J95" t="n">
-        <v>2555.67079999999987</v>
+        <v>2.92820109999999989</v>
       </c>
       <c r="K95" t="n">
-        <v>2.92820109999999989</v>
-      </c>
-      <c r="L95" t="n">
         <v>620.799999999999955</v>
       </c>
     </row>
-    <row r="96" spans="1:18">
+    <row r="96" spans="1:12">
       <c r="A96" t="n">
         <v>32257</v>
       </c>
@@ -4146,37 +3859,34 @@
         <v>5.66878420000000016</v>
       </c>
       <c r="C96" t="n">
-        <v>7.60606359999999881</v>
+        <v>7.6060635999999997</v>
       </c>
       <c r="D96" t="n">
         <v>5422.51860000000033</v>
       </c>
       <c r="E96" t="n">
-        <v>20421211</v>
+        <v>4017.75</v>
       </c>
       <c r="F96" t="n">
-        <v>4017.75</v>
+        <v>9.51860280000000003</v>
       </c>
       <c r="G96" t="n">
-        <v>9.51860280000000003</v>
+        <v>49.8732960000000034</v>
       </c>
       <c r="H96" t="n">
-        <v>49.8732960000000034</v>
+        <v>1974.27690000000007</v>
       </c>
       <c r="I96" t="n">
-        <v>1974.27690000000007</v>
+        <v>1926.04449999999997</v>
       </c>
       <c r="J96" t="n">
-        <v>1926.04449999999997</v>
+        <v>2.17000029999999988</v>
       </c>
       <c r="K96" t="n">
-        <v>2.17000029999999988</v>
-      </c>
-      <c r="L96" t="n">
         <v>772.200000000000045</v>
       </c>
     </row>
-    <row r="97" spans="1:18">
+    <row r="97" spans="1:12">
       <c r="A97" t="n">
         <v>32257</v>
       </c>
@@ -4190,31 +3900,28 @@
         <v>5356.80280000000039</v>
       </c>
       <c r="E97" t="n">
-        <v>20411227</v>
+        <v>3652.5</v>
       </c>
       <c r="F97" t="n">
-        <v>3652.5</v>
+        <v>11.6581840000000003</v>
       </c>
       <c r="G97" t="n">
-        <v>11.6581840000000003</v>
+        <v>49.3356640000000013</v>
       </c>
       <c r="H97" t="n">
-        <v>49.3356640000000013</v>
+        <v>1416.85069999999996</v>
       </c>
       <c r="I97" t="n">
-        <v>1416.85069999999996</v>
+        <v>2396.55850000000009</v>
       </c>
       <c r="J97" t="n">
-        <v>2396.55850000000009</v>
+        <v>3.15556700000000001</v>
       </c>
       <c r="K97" t="n">
-        <v>3.15556700000000001</v>
-      </c>
-      <c r="L97" t="n">
-        <v>793.399999999999977</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18">
+        <v>793.399999999999864</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98" t="n">
         <v>32257</v>
       </c>
@@ -4228,31 +3935,28 @@
         <v>5263.94459999999981</v>
       </c>
       <c r="E98" t="n">
-        <v>20411215</v>
+        <v>4017.75</v>
       </c>
       <c r="F98" t="n">
-        <v>4017.75</v>
+        <v>10.9771190000000001</v>
       </c>
       <c r="G98" t="n">
-        <v>10.9771190000000001</v>
+        <v>47.0779970000000034</v>
       </c>
       <c r="H98" t="n">
-        <v>47.0779970000000034</v>
+        <v>1640.03760000000011</v>
       </c>
       <c r="I98" t="n">
-        <v>1640.03760000000011</v>
+        <v>2339.1244999999999</v>
       </c>
       <c r="J98" t="n">
-        <v>2339.1244999999999</v>
+        <v>2.82494710000000016</v>
       </c>
       <c r="K98" t="n">
-        <v>2.82494710000000016</v>
-      </c>
-      <c r="L98" t="n">
         <v>534.799999999999955</v>
       </c>
     </row>
-    <row r="99" spans="1:18">
+    <row r="99" spans="1:12">
       <c r="A99" t="n">
         <v>32257</v>
       </c>
@@ -4266,31 +3970,28 @@
         <v>5150.42479999999978</v>
       </c>
       <c r="E99" t="n">
-        <v>20401225</v>
+        <v>3652.5</v>
       </c>
       <c r="F99" t="n">
-        <v>3652.5</v>
+        <v>13.4276180000000007</v>
       </c>
       <c r="G99" t="n">
-        <v>13.4276180000000007</v>
+        <v>47.5418239999999983</v>
       </c>
       <c r="H99" t="n">
-        <v>47.5418239999999983</v>
+        <v>1075.67599999999993</v>
       </c>
       <c r="I99" t="n">
-        <v>1075.67599999999993</v>
+        <v>2796.73050000000012</v>
       </c>
       <c r="J99" t="n">
-        <v>2796.73050000000012</v>
+        <v>4.08252039999999994</v>
       </c>
       <c r="K99" t="n">
-        <v>4.08252039999999994</v>
-      </c>
-      <c r="L99" t="n">
         <v>528</v>
       </c>
     </row>
-    <row r="100" spans="1:18">
+    <row r="100" spans="1:12">
       <c r="A100" t="n">
         <v>32257</v>
       </c>
@@ -4304,31 +4005,28 @@
         <v>5390.28949999999986</v>
       </c>
       <c r="E100" t="n">
-        <v>20421004</v>
+        <v>4017.75</v>
       </c>
       <c r="F100" t="n">
-        <v>4017.75</v>
+        <v>9.87046780000000012</v>
       </c>
       <c r="G100" t="n">
-        <v>9.87046780000000012</v>
+        <v>49.6702859999999973</v>
       </c>
       <c r="H100" t="n">
-        <v>49.6702859999999973</v>
+        <v>1840.44830000000002</v>
       </c>
       <c r="I100" t="n">
-        <v>1840.44830000000002</v>
+        <v>1972.0628999999999</v>
       </c>
       <c r="J100" t="n">
-        <v>1972.0628999999999</v>
+        <v>2.32114229999999999</v>
       </c>
       <c r="K100" t="n">
-        <v>2.32114229999999999</v>
-      </c>
-      <c r="L100" t="n">
-        <v>827.799999999999955</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18">
+        <v>827.799999999999841</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
       <c r="A101" t="n">
         <v>32257</v>
       </c>
@@ -4342,31 +4040,28 @@
         <v>4408.50540000000001</v>
       </c>
       <c r="E101" t="n">
-        <v>20410905</v>
+        <v>3652.5</v>
       </c>
       <c r="F101" t="n">
-        <v>3652.5</v>
+        <v>11.9572310000000002</v>
       </c>
       <c r="G101" t="n">
-        <v>11.9572310000000002</v>
+        <v>47.7919709999999966</v>
       </c>
       <c r="H101" t="n">
-        <v>47.7919709999999966</v>
+        <v>1112.52819999999997</v>
       </c>
       <c r="I101" t="n">
-        <v>1112.52819999999997</v>
+        <v>2026.01309999999989</v>
       </c>
       <c r="J101" t="n">
-        <v>2026.01309999999989</v>
+        <v>3.30547840000000015</v>
       </c>
       <c r="K101" t="n">
-        <v>3.30547840000000015</v>
-      </c>
-      <c r="L101" t="n">
         <v>520</v>
       </c>
     </row>
-    <row r="102" spans="1:18">
+    <row r="102" spans="1:12">
       <c r="A102" t="n">
         <v>32257</v>
       </c>
@@ -4380,31 +4075,28 @@
         <v>5548.89590000000044</v>
       </c>
       <c r="E102" t="n">
-        <v>20430227</v>
+        <v>4017.75</v>
       </c>
       <c r="F102" t="n">
-        <v>4017.75</v>
+        <v>9.10679619999999979</v>
       </c>
       <c r="G102" t="n">
-        <v>9.10679619999999979</v>
+        <v>49.9580320000000029</v>
       </c>
       <c r="H102" t="n">
-        <v>49.9580320000000029</v>
+        <v>2173.81880000000001</v>
       </c>
       <c r="I102" t="n">
-        <v>2173.81880000000001</v>
+        <v>1896.18579999999997</v>
       </c>
       <c r="J102" t="n">
-        <v>1896.18579999999997</v>
+        <v>1.99885580000000012</v>
       </c>
       <c r="K102" t="n">
-        <v>1.99885580000000012</v>
-      </c>
-      <c r="L102" t="n">
-        <v>728.899999999999977</v>
-      </c>
-    </row>
-    <row r="103" spans="1:18">
+        <v>728.899999999999864</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
       <c r="A103" t="n">
         <v>32257</v>
       </c>
@@ -4418,31 +4110,28 @@
         <v>5411.35869999999977</v>
       </c>
       <c r="E103" t="n">
-        <v>20420324</v>
+        <v>3652.5</v>
       </c>
       <c r="F103" t="n">
-        <v>3652.5</v>
+        <v>11.0424849999999992</v>
       </c>
       <c r="G103" t="n">
-        <v>11.0424849999999992</v>
+        <v>49.3751869999999968</v>
       </c>
       <c r="H103" t="n">
-        <v>49.3751869999999968</v>
+        <v>1618.32249999999999</v>
       </c>
       <c r="I103" t="n">
-        <v>1618.32249999999999</v>
+        <v>2346.61529999999993</v>
       </c>
       <c r="J103" t="n">
-        <v>2346.61529999999993</v>
+        <v>2.85601540000000007</v>
       </c>
       <c r="K103" t="n">
-        <v>2.85601540000000007</v>
-      </c>
-      <c r="L103" t="n">
         <v>696.399999999999977</v>
       </c>
     </row>
-    <row r="104" spans="1:18">
+    <row r="104" spans="1:12">
       <c r="A104" t="n">
         <v>32257</v>
       </c>
@@ -4456,31 +4145,28 @@
         <v>5125.83640000000014</v>
       </c>
       <c r="E104" t="n">
-        <v>20430225</v>
+        <v>4017.75</v>
       </c>
       <c r="F104" t="n">
-        <v>4017.75</v>
+        <v>9.13039419999999957</v>
       </c>
       <c r="G104" t="n">
-        <v>9.13039419999999957</v>
+        <v>50.0301389999999984</v>
       </c>
       <c r="H104" t="n">
-        <v>50.0301389999999984</v>
+        <v>1965.79970000000003</v>
       </c>
       <c r="I104" t="n">
-        <v>1965.79970000000003</v>
+        <v>1725.88040000000001</v>
       </c>
       <c r="J104" t="n">
-        <v>1725.88040000000001</v>
+        <v>2.00849339999999987</v>
       </c>
       <c r="K104" t="n">
-        <v>2.00849339999999987</v>
-      </c>
-      <c r="L104" t="n">
         <v>684.200000000000045</v>
       </c>
     </row>
-    <row r="105" spans="1:18">
+    <row r="105" spans="1:12">
       <c r="A105" t="n">
         <v>32257</v>
       </c>
@@ -4494,31 +4180,28 @@
         <v>5104.63490000000002</v>
       </c>
       <c r="E105" t="n">
-        <v>20420301</v>
+        <v>3652.5</v>
       </c>
       <c r="F105" t="n">
-        <v>3652.5</v>
+        <v>11.2165649999999992</v>
       </c>
       <c r="G105" t="n">
-        <v>11.2165649999999992</v>
+        <v>49.4129179999999977</v>
       </c>
       <c r="H105" t="n">
-        <v>49.4129179999999977</v>
+        <v>1453.12120000000004</v>
       </c>
       <c r="I105" t="n">
-        <v>1453.12120000000004</v>
+        <v>2201.49699999999984</v>
       </c>
       <c r="J105" t="n">
-        <v>2201.49699999999984</v>
+        <v>2.9394480999999999</v>
       </c>
       <c r="K105" t="n">
-        <v>2.9394480999999999</v>
-      </c>
-      <c r="L105" t="n">
         <v>700</v>
       </c>
     </row>
-    <row r="106" spans="1:18">
+    <row r="106" spans="1:12">
       <c r="A106" t="n">
         <v>32257</v>
       </c>
@@ -4532,31 +4215,28 @@
         <v>4069.61400000000003</v>
       </c>
       <c r="E106" t="n">
-        <v>20430802</v>
+        <v>4017.75</v>
       </c>
       <c r="F106" t="n">
-        <v>4017.75</v>
+        <v>8.39226580000000055</v>
       </c>
       <c r="G106" t="n">
-        <v>8.39226580000000055</v>
+        <v>50.411645</v>
       </c>
       <c r="H106" t="n">
-        <v>50.411645</v>
+        <v>1648.75990000000002</v>
       </c>
       <c r="I106" t="n">
-        <v>1648.75990000000002</v>
+        <v>1176.92419999999993</v>
       </c>
       <c r="J106" t="n">
-        <v>1176.92419999999993</v>
+        <v>1.71701009999999998</v>
       </c>
       <c r="K106" t="n">
-        <v>1.71701009999999998</v>
-      </c>
-      <c r="L106" t="n">
         <v>493.899999999999977</v>
       </c>
     </row>
-    <row r="107" spans="1:18">
+    <row r="107" spans="1:12">
       <c r="A107" t="n">
         <v>32257</v>
       </c>
@@ -4570,31 +4250,28 @@
         <v>4132.80839999999989</v>
       </c>
       <c r="E107" t="n">
-        <v>20430929</v>
+        <v>4017.75</v>
       </c>
       <c r="F107" t="n">
-        <v>4017.75</v>
+        <v>8.13408790000000081</v>
       </c>
       <c r="G107" t="n">
-        <v>8.13408790000000081</v>
+        <v>50.490988999999999</v>
       </c>
       <c r="H107" t="n">
-        <v>50.490988999999999</v>
+        <v>1728.6887999999999</v>
       </c>
       <c r="I107" t="n">
-        <v>1728.6887999999999</v>
+        <v>1145.16499999999996</v>
       </c>
       <c r="J107" t="n">
-        <v>1145.16499999999996</v>
+        <v>1.62000440000000001</v>
       </c>
       <c r="K107" t="n">
-        <v>1.62000440000000001</v>
-      </c>
-      <c r="L107" t="n">
         <v>509</v>
       </c>
     </row>
-    <row r="108" spans="1:18">
+    <row r="108" spans="1:12">
       <c r="A108" t="n">
         <v>32257</v>
       </c>
@@ -4602,37 +4279,34 @@
         <v>20.511412</v>
       </c>
       <c r="C108" t="n">
-        <v>11.6253229999999999</v>
+        <v>11.6253230000000016</v>
       </c>
       <c r="D108" t="n">
         <v>4035.8152</v>
       </c>
       <c r="E108" t="n">
-        <v>20411011</v>
+        <v>3287.25</v>
       </c>
       <c r="F108" t="n">
-        <v>3287.25</v>
+        <v>12.2074649999999991</v>
       </c>
       <c r="G108" t="n">
-        <v>12.2074649999999991</v>
+        <v>49.1917710000000028</v>
       </c>
       <c r="H108" t="n">
-        <v>49.1917710000000028</v>
+        <v>950.794300000000021</v>
       </c>
       <c r="I108" t="n">
-        <v>950.794300000000021</v>
+        <v>1841.05340000000001</v>
       </c>
       <c r="J108" t="n">
-        <v>1841.05340000000001</v>
+        <v>3.43308629999999981</v>
       </c>
       <c r="K108" t="n">
-        <v>3.43308629999999981</v>
-      </c>
-      <c r="L108" t="n">
         <v>494</v>
       </c>
     </row>
-    <row r="109" spans="1:18">
+    <row r="109" spans="1:12">
       <c r="A109" t="n">
         <v>32257</v>
       </c>
@@ -4646,27 +4320,24 @@
         <v>4111.32949999999983</v>
       </c>
       <c r="E109" t="n">
-        <v>20421001</v>
+        <v>3652.5</v>
       </c>
       <c r="F109" t="n">
-        <v>3652.5</v>
+        <v>9.88747500000000024</v>
       </c>
       <c r="G109" t="n">
-        <v>9.88747500000000024</v>
+        <v>49.6688240000000008</v>
       </c>
       <c r="H109" t="n">
-        <v>49.6688240000000008</v>
+        <v>1375.70890000000009</v>
       </c>
       <c r="I109" t="n">
-        <v>1375.70890000000009</v>
+        <v>1480.72970000000009</v>
       </c>
       <c r="J109" t="n">
-        <v>1480.72970000000009</v>
+        <v>2.32856059999999987</v>
       </c>
       <c r="K109" t="n">
-        <v>2.32856059999999987</v>
-      </c>
-      <c r="L109" t="n">
         <v>504.899999999999977</v>
       </c>
     </row>
@@ -4674,7 +4345,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1591621747" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1591622550" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4683,8 +4354,8 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1591621747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1591621747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1591622550" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1591622550" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
@@ -4693,7 +4364,7 @@
   </tableParts>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1591621747" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1591622550" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>